<commit_message>
Update picture pull table
</commit_message>
<xml_diff>
--- a/R/processed_data/picturePulls.xlsx
+++ b/R/processed_data/picturePulls.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t xml:space="preserve">pic_id</t>
   </si>
@@ -44,7 +44,10 @@
     <t xml:space="preserve">pow.meanPresent</t>
   </si>
   <si>
-    <t xml:space="preserve">overallPull</t>
+    <t xml:space="preserve">overall.mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">overall.sd</t>
   </si>
   <si>
     <t xml:space="preserve">sc.mean</t>
@@ -611,10 +614,13 @@
       <c r="R1" t="s">
         <v>17</v>
       </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" t="n">
         <v>1.88</v>
@@ -647,30 +653,33 @@
         <v>4.47</v>
       </c>
       <c r="L2" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="M2" t="n">
         <v>6.39</v>
       </c>
-      <c r="M2" t="n">
+      <c r="N2" t="n">
         <v>2.77</v>
       </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
         <v>90.28</v>
       </c>
-      <c r="O2" t="n">
+      <c r="P2" t="n">
         <v>34.11</v>
       </c>
-      <c r="P2" t="n">
+      <c r="Q2" t="n">
         <v>0.59</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="R2" t="n">
         <v>0.91</v>
       </c>
-      <c r="R2" t="n">
+      <c r="S2" t="n">
         <v>1195</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="n">
         <v>2.23</v>
@@ -703,30 +712,33 @@
         <v>3.2</v>
       </c>
       <c r="L3" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="M3" t="n">
         <v>7.32</v>
       </c>
-      <c r="M3" t="n">
+      <c r="N3" t="n">
         <v>3.34</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>106.57</v>
       </c>
-      <c r="O3" t="n">
+      <c r="P3" t="n">
         <v>35.27</v>
       </c>
-      <c r="P3" t="n">
+      <c r="Q3" t="n">
         <v>0.38</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="R3" t="n">
         <v>0.8</v>
       </c>
-      <c r="R3" t="n">
+      <c r="S3" t="n">
         <v>408</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" t="n">
         <v>0.62</v>
@@ -759,30 +771,33 @@
         <v>4.17</v>
       </c>
       <c r="L4" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="M4" t="n">
         <v>6.77</v>
       </c>
-      <c r="M4" t="n">
+      <c r="N4" t="n">
         <v>2.89</v>
       </c>
-      <c r="N4" t="n">
+      <c r="O4" t="n">
         <v>97.07</v>
       </c>
-      <c r="O4" t="n">
+      <c r="P4" t="n">
         <v>34.25</v>
       </c>
-      <c r="P4" t="n">
+      <c r="Q4" t="n">
         <v>0.75</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="R4" t="n">
         <v>0.96</v>
       </c>
-      <c r="R4" t="n">
+      <c r="S4" t="n">
         <v>797</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" t="n">
         <v>0.13</v>
@@ -815,30 +830,33 @@
         <v>4.24</v>
       </c>
       <c r="L5" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="M5" t="n">
         <v>7.52</v>
       </c>
-      <c r="M5" t="n">
+      <c r="N5" t="n">
         <v>4.61</v>
       </c>
-      <c r="N5" t="n">
+      <c r="O5" t="n">
         <v>97.2</v>
       </c>
-      <c r="O5" t="n">
+      <c r="P5" t="n">
         <v>62.22</v>
       </c>
-      <c r="P5" t="n">
+      <c r="Q5" t="n">
         <v>1.11</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="R5" t="n">
         <v>1.46</v>
       </c>
-      <c r="R5" t="n">
+      <c r="S5" t="n">
         <v>83</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="n">
         <v>0.34</v>
@@ -871,30 +889,33 @@
         <v>2.83</v>
       </c>
       <c r="L6" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="M6" t="n">
         <v>7.19</v>
       </c>
-      <c r="M6" t="n">
+      <c r="N6" t="n">
         <v>3.58</v>
       </c>
-      <c r="N6" t="n">
+      <c r="O6" t="n">
         <v>88.56</v>
       </c>
-      <c r="O6" t="n">
+      <c r="P6" t="n">
         <v>36.86</v>
       </c>
-      <c r="P6" t="n">
+      <c r="Q6" t="n">
         <v>0.67</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="R6" t="n">
         <v>1.02</v>
       </c>
-      <c r="R6" t="n">
+      <c r="S6" t="n">
         <v>1724</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" t="n">
         <v>2.04</v>
@@ -927,30 +948,33 @@
         <v>3.44</v>
       </c>
       <c r="L7" t="n">
+        <v>2.34</v>
+      </c>
+      <c r="M7" t="n">
         <v>7.33</v>
       </c>
-      <c r="M7" t="n">
+      <c r="N7" t="n">
         <v>3.2</v>
       </c>
-      <c r="N7" t="n">
+      <c r="O7" t="n">
         <v>92.48</v>
       </c>
-      <c r="O7" t="n">
+      <c r="P7" t="n">
         <v>30.97</v>
       </c>
-      <c r="P7" t="n">
+      <c r="Q7" t="n">
         <v>0.98</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="R7" t="n">
         <v>1.31</v>
       </c>
-      <c r="R7" t="n">
+      <c r="S7" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" t="n">
         <v>0.68</v>
@@ -983,30 +1007,33 @@
         <v>1.76</v>
       </c>
       <c r="L8" t="n">
+        <v>1.87</v>
+      </c>
+      <c r="M8" t="n">
         <v>6.65</v>
       </c>
-      <c r="M8" t="n">
+      <c r="N8" t="n">
         <v>4.8</v>
       </c>
-      <c r="N8" t="n">
+      <c r="O8" t="n">
         <v>81.32</v>
       </c>
-      <c r="O8" t="n">
+      <c r="P8" t="n">
         <v>43.68</v>
       </c>
-      <c r="P8" t="n">
+      <c r="Q8" t="n">
         <v>0.59</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="R8" t="n">
         <v>0.9</v>
       </c>
-      <c r="R8" t="n">
+      <c r="S8" t="n">
         <v>111</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" t="n">
         <v>3.03</v>
@@ -1039,30 +1066,33 @@
         <v>3.41</v>
       </c>
       <c r="L9" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="M9" t="n">
         <v>7.08</v>
       </c>
-      <c r="M9" t="n">
+      <c r="N9" t="n">
         <v>3.57</v>
       </c>
-      <c r="N9" t="n">
+      <c r="O9" t="n">
         <v>94.25</v>
       </c>
-      <c r="O9" t="n">
+      <c r="P9" t="n">
         <v>40.16</v>
       </c>
-      <c r="P9" t="n">
+      <c r="Q9" t="n">
         <v>0.72</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="R9" t="n">
         <v>1.11</v>
       </c>
-      <c r="R9" t="n">
+      <c r="S9" t="n">
         <v>1854</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" t="n">
         <v>0.85</v>
@@ -1095,30 +1125,33 @@
         <v>2.18</v>
       </c>
       <c r="L10" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="M10" t="n">
         <v>6.88</v>
       </c>
-      <c r="M10" t="n">
+      <c r="N10" t="n">
         <v>3.88</v>
       </c>
-      <c r="N10" t="n">
+      <c r="O10" t="n">
         <v>88.97</v>
       </c>
-      <c r="O10" t="n">
+      <c r="P10" t="n">
         <v>40.26</v>
       </c>
-      <c r="P10" t="n">
+      <c r="Q10" t="n">
         <v>0.79</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="R10" t="n">
         <v>1.08</v>
       </c>
-      <c r="R10" t="n">
+      <c r="S10" t="n">
         <v>125</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" t="n">
         <v>0.1</v>
@@ -1151,30 +1184,33 @@
         <v>3.22</v>
       </c>
       <c r="L11" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="M11" t="n">
         <v>5.94</v>
       </c>
-      <c r="M11" t="n">
+      <c r="N11" t="n">
         <v>2.67</v>
       </c>
-      <c r="N11" t="n">
+      <c r="O11" t="n">
         <v>84.96</v>
       </c>
-      <c r="O11" t="n">
+      <c r="P11" t="n">
         <v>31.05</v>
       </c>
-      <c r="P11" t="n">
+      <c r="Q11" t="n">
         <v>0.44</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="R11" t="n">
         <v>0.74</v>
       </c>
-      <c r="R11" t="n">
+      <c r="S11" t="n">
         <v>799</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" t="n">
         <v>0.2</v>
@@ -1207,30 +1243,33 @@
         <v>2.44</v>
       </c>
       <c r="L12" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="M12" t="n">
         <v>6.86</v>
       </c>
-      <c r="M12" t="n">
+      <c r="N12" t="n">
         <v>3.12</v>
       </c>
-      <c r="N12" t="n">
+      <c r="O12" t="n">
         <v>92.34</v>
       </c>
-      <c r="O12" t="n">
+      <c r="P12" t="n">
         <v>36</v>
       </c>
-      <c r="P12" t="n">
+      <c r="Q12" t="n">
         <v>0.73</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="R12" t="n">
         <v>0.98</v>
       </c>
-      <c r="R12" t="n">
+      <c r="S12" t="n">
         <v>97</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" t="n">
         <v>0.08</v>
@@ -1263,30 +1302,33 @@
         <v>1.18</v>
       </c>
       <c r="L13" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="M13" t="n">
         <v>5.98</v>
       </c>
-      <c r="M13" t="n">
+      <c r="N13" t="n">
         <v>2.71</v>
       </c>
-      <c r="N13" t="n">
+      <c r="O13" t="n">
         <v>86.08</v>
       </c>
-      <c r="O13" t="n">
+      <c r="P13" t="n">
         <v>27.11</v>
       </c>
-      <c r="P13" t="n">
+      <c r="Q13" t="n">
         <v>0.36</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="R13" t="n">
         <v>0.73</v>
       </c>
-      <c r="R13" t="n">
+      <c r="S13" t="n">
         <v>95</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" t="n">
         <v>0.49</v>
@@ -1319,30 +1361,33 @@
         <v>2.16</v>
       </c>
       <c r="L14" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="M14" t="n">
         <v>6</v>
       </c>
-      <c r="M14" t="n">
+      <c r="N14" t="n">
         <v>2.5</v>
       </c>
-      <c r="N14" t="n">
+      <c r="O14" t="n">
         <v>82.48</v>
       </c>
-      <c r="O14" t="n">
+      <c r="P14" t="n">
         <v>35.08</v>
       </c>
-      <c r="P14" t="n">
+      <c r="Q14" t="n">
         <v>0.98</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="R14" t="n">
         <v>1.18</v>
       </c>
-      <c r="R14" t="n">
+      <c r="S14" t="n">
         <v>202</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" t="n">
         <v>1.71</v>
@@ -1375,30 +1420,33 @@
         <v>3.32</v>
       </c>
       <c r="L15" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="M15" t="n">
         <v>6.54</v>
       </c>
-      <c r="M15" t="n">
+      <c r="N15" t="n">
         <v>2.7</v>
       </c>
-      <c r="N15" t="n">
+      <c r="O15" t="n">
         <v>86.97</v>
       </c>
-      <c r="O15" t="n">
+      <c r="P15" t="n">
         <v>34.91</v>
       </c>
-      <c r="P15" t="n">
+      <c r="Q15" t="n">
         <v>0.35</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="R15" t="n">
         <v>0.59</v>
       </c>
-      <c r="R15" t="n">
+      <c r="S15" t="n">
         <v>196</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" t="n">
         <v>0.4</v>
@@ -1431,30 +1479,33 @@
         <v>2.8</v>
       </c>
       <c r="L16" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="M16" t="n">
         <v>6.8</v>
       </c>
-      <c r="M16" t="n">
+      <c r="N16" t="n">
         <v>3.91</v>
       </c>
-      <c r="N16" t="n">
+      <c r="O16" t="n">
         <v>87.1</v>
       </c>
-      <c r="O16" t="n">
+      <c r="P16" t="n">
         <v>51.74</v>
       </c>
-      <c r="P16" t="n">
+      <c r="Q16" t="n">
         <v>1.2</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="R16" t="n">
         <v>1.4</v>
       </c>
-      <c r="R16" t="n">
+      <c r="S16" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" t="n">
         <v>0.55</v>
@@ -1487,30 +1538,33 @@
         <v>2.63</v>
       </c>
       <c r="L17" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="M17" t="n">
         <v>6.33</v>
       </c>
-      <c r="M17" t="n">
+      <c r="N17" t="n">
         <v>2.83</v>
       </c>
-      <c r="N17" t="n">
+      <c r="O17" t="n">
         <v>82.91</v>
       </c>
-      <c r="O17" t="n">
+      <c r="P17" t="n">
         <v>33.61</v>
       </c>
-      <c r="P17" t="n">
+      <c r="Q17" t="n">
         <v>0.65</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="R17" t="n">
         <v>0.95</v>
       </c>
-      <c r="R17" t="n">
+      <c r="S17" t="n">
         <v>196</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" t="n">
         <v>1.18</v>
@@ -1543,30 +1597,33 @@
         <v>2.18</v>
       </c>
       <c r="L18" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="M18" t="n">
         <v>6.18</v>
       </c>
-      <c r="M18" t="n">
+      <c r="N18" t="n">
         <v>3.49</v>
       </c>
-      <c r="N18" t="n">
+      <c r="O18" t="n">
         <v>74.73</v>
       </c>
-      <c r="O18" t="n">
+      <c r="P18" t="n">
         <v>32.6</v>
       </c>
-      <c r="P18" t="n">
+      <c r="Q18" t="n">
         <v>0.45</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="R18" t="n">
         <v>0.69</v>
       </c>
-      <c r="R18" t="n">
+      <c r="S18" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" t="n">
         <v>1.88</v>
@@ -1599,30 +1656,33 @@
         <v>3.25</v>
       </c>
       <c r="L19" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="M19" t="n">
         <v>9.75</v>
       </c>
-      <c r="M19" t="n">
+      <c r="N19" t="n">
         <v>4.2</v>
       </c>
-      <c r="N19" t="n">
+      <c r="O19" t="n">
         <v>100</v>
       </c>
-      <c r="O19" t="n">
+      <c r="P19" t="n">
         <v>45.3</v>
       </c>
-      <c r="P19" t="n">
+      <c r="Q19" t="n">
         <v>1.5</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="R19" t="n">
         <v>0.93</v>
       </c>
-      <c r="R19" t="n">
+      <c r="S19" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" t="n">
         <v>1.29</v>
@@ -1655,30 +1715,33 @@
         <v>2.71</v>
       </c>
       <c r="L20" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="M20" t="n">
         <v>6.29</v>
       </c>
-      <c r="M20" t="n">
+      <c r="N20" t="n">
         <v>2.81</v>
       </c>
-      <c r="N20" t="n">
+      <c r="O20" t="n">
         <v>84.29</v>
       </c>
-      <c r="O20" t="n">
+      <c r="P20" t="n">
         <v>30.61</v>
       </c>
-      <c r="P20" t="n">
+      <c r="Q20" t="n">
         <v>1.43</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="R20" t="n">
         <v>1.51</v>
       </c>
-      <c r="R20" t="n">
+      <c r="S20" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" t="n">
         <v>0.09</v>
@@ -1711,30 +1774,33 @@
         <v>3.27</v>
       </c>
       <c r="L21" t="n">
+        <v>1.79</v>
+      </c>
+      <c r="M21" t="n">
         <v>7.64</v>
       </c>
-      <c r="M21" t="n">
+      <c r="N21" t="n">
         <v>2.06</v>
       </c>
-      <c r="N21" t="n">
+      <c r="O21" t="n">
         <v>73.73</v>
       </c>
-      <c r="O21" t="n">
+      <c r="P21" t="n">
         <v>28.44</v>
       </c>
-      <c r="P21" t="n">
+      <c r="Q21" t="n">
         <v>0.55</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="R21" t="n">
         <v>0.93</v>
       </c>
-      <c r="R21" t="n">
+      <c r="S21" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" t="n">
         <v>3.25</v>
@@ -1767,30 +1833,33 @@
         <v>4.5</v>
       </c>
       <c r="L22" t="n">
+        <v>3</v>
+      </c>
+      <c r="M22" t="n">
         <v>10.5</v>
       </c>
-      <c r="M22" t="n">
+      <c r="N22" t="n">
         <v>3.7</v>
       </c>
-      <c r="N22" t="n">
+      <c r="O22" t="n">
         <v>118.5</v>
       </c>
-      <c r="O22" t="n">
+      <c r="P22" t="n">
         <v>31.08</v>
       </c>
-      <c r="P22" t="n">
+      <c r="Q22" t="n">
         <v>1.25</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="R22" t="n">
         <v>1.26</v>
       </c>
-      <c r="R22" t="n">
+      <c r="S22" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" t="n">
         <v>1.75</v>
@@ -1823,30 +1892,33 @@
         <v>2.5</v>
       </c>
       <c r="L23" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="M23" t="n">
         <v>6.25</v>
       </c>
-      <c r="M23" t="n">
+      <c r="N23" t="n">
         <v>4.5</v>
       </c>
-      <c r="N23" t="n">
+      <c r="O23" t="n">
         <v>73.38</v>
       </c>
-      <c r="O23" t="n">
+      <c r="P23" t="n">
         <v>44.11</v>
       </c>
-      <c r="P23" t="n">
+      <c r="Q23" t="n">
         <v>0.25</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="R23" t="n">
         <v>0.46</v>
       </c>
-      <c r="R23" t="n">
+      <c r="S23" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" t="n">
         <v>1.89</v>
@@ -1879,30 +1951,33 @@
         <v>2.56</v>
       </c>
       <c r="L24" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="M24" t="n">
         <v>8.22</v>
       </c>
-      <c r="M24" t="n">
+      <c r="N24" t="n">
         <v>5.7</v>
       </c>
-      <c r="N24" t="n">
+      <c r="O24" t="n">
         <v>92.22</v>
       </c>
-      <c r="O24" t="n">
+      <c r="P24" t="n">
         <v>35.45</v>
       </c>
-      <c r="P24" t="n">
+      <c r="Q24" t="n">
         <v>0.67</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="R24" t="n">
         <v>1</v>
       </c>
-      <c r="R24" t="n">
+      <c r="S24" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" t="n">
         <v>0.46</v>
@@ -1935,30 +2010,33 @@
         <v>2.5</v>
       </c>
       <c r="L25" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="M25" t="n">
         <v>6.39</v>
       </c>
-      <c r="M25" t="n">
+      <c r="N25" t="n">
         <v>2.68</v>
       </c>
-      <c r="N25" t="n">
+      <c r="O25" t="n">
         <v>78.2</v>
       </c>
-      <c r="O25" t="n">
+      <c r="P25" t="n">
         <v>34.44</v>
       </c>
-      <c r="P25" t="n">
+      <c r="Q25" t="n">
         <v>0.42</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="R25" t="n">
         <v>0.74</v>
       </c>
-      <c r="R25" t="n">
+      <c r="S25" t="n">
         <v>200</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" t="n">
         <v>0.62</v>
@@ -1991,30 +2069,33 @@
         <v>2.38</v>
       </c>
       <c r="L26" t="n">
+        <v>2.45</v>
+      </c>
+      <c r="M26" t="n">
         <v>7.5</v>
       </c>
-      <c r="M26" t="n">
+      <c r="N26" t="n">
         <v>4.84</v>
       </c>
-      <c r="N26" t="n">
+      <c r="O26" t="n">
         <v>85.38</v>
       </c>
-      <c r="O26" t="n">
+      <c r="P26" t="n">
         <v>38.78</v>
       </c>
-      <c r="P26" t="n">
+      <c r="Q26" t="n">
         <v>1</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="R26" t="n">
         <v>2.07</v>
       </c>
-      <c r="R26" t="n">
+      <c r="S26" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" t="n">
         <v>0.77</v>
@@ -2047,30 +2128,33 @@
         <v>3.15</v>
       </c>
       <c r="L27" t="n">
+        <v>3.11</v>
+      </c>
+      <c r="M27" t="n">
         <v>9.46</v>
       </c>
-      <c r="M27" t="n">
+      <c r="N27" t="n">
         <v>4.03</v>
       </c>
-      <c r="N27" t="n">
+      <c r="O27" t="n">
         <v>103.92</v>
       </c>
-      <c r="O27" t="n">
+      <c r="P27" t="n">
         <v>39.52</v>
       </c>
-      <c r="P27" t="n">
+      <c r="Q27" t="n">
         <v>1.23</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="R27" t="n">
         <v>1.09</v>
       </c>
-      <c r="R27" t="n">
+      <c r="S27" t="n">
         <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" t="n">
         <v>2.18</v>
@@ -2103,30 +2187,33 @@
         <v>3.45</v>
       </c>
       <c r="L28" t="n">
+        <v>2.16</v>
+      </c>
+      <c r="M28" t="n">
         <v>7.45</v>
       </c>
-      <c r="M28" t="n">
+      <c r="N28" t="n">
         <v>2.62</v>
       </c>
-      <c r="N28" t="n">
+      <c r="O28" t="n">
         <v>92.09</v>
       </c>
-      <c r="O28" t="n">
+      <c r="P28" t="n">
         <v>41.49</v>
       </c>
-      <c r="P28" t="n">
+      <c r="Q28" t="n">
         <v>1.09</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="R28" t="n">
         <v>1.81</v>
       </c>
-      <c r="R28" t="n">
+      <c r="S28" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" t="n">
         <v>0.67</v>
@@ -2159,30 +2246,33 @@
         <v>1</v>
       </c>
       <c r="L29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M29" t="n">
         <v>6.33</v>
       </c>
-      <c r="M29" t="n">
+      <c r="N29" t="n">
         <v>3.51</v>
       </c>
-      <c r="N29" t="n">
+      <c r="O29" t="n">
         <v>82.67</v>
       </c>
-      <c r="O29" t="n">
+      <c r="P29" t="n">
         <v>59.35</v>
       </c>
-      <c r="P29" t="n">
+      <c r="Q29" t="n">
         <v>0.33</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="R29" t="n">
         <v>0.58</v>
       </c>
-      <c r="R29" t="n">
+      <c r="S29" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" t="n">
         <v>2.33</v>
@@ -2215,30 +2305,33 @@
         <v>3.33</v>
       </c>
       <c r="L30" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="M30" t="n">
         <v>10</v>
       </c>
-      <c r="M30" t="n">
+      <c r="N30" t="n">
         <v>4.58</v>
       </c>
-      <c r="N30" t="n">
+      <c r="O30" t="n">
         <v>113.33</v>
       </c>
-      <c r="O30" t="n">
+      <c r="P30" t="n">
         <v>55.9</v>
-      </c>
-      <c r="P30" t="n">
-        <v>1</v>
       </c>
       <c r="Q30" t="n">
         <v>1</v>
       </c>
       <c r="R30" t="n">
+        <v>1</v>
+      </c>
+      <c r="S30" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" t="n">
         <v>1.2</v>
@@ -2271,30 +2364,33 @@
         <v>1.93</v>
       </c>
       <c r="L31" t="n">
+        <v>1.39</v>
+      </c>
+      <c r="M31" t="n">
         <v>6.93</v>
       </c>
-      <c r="M31" t="n">
+      <c r="N31" t="n">
         <v>3.59</v>
       </c>
-      <c r="N31" t="n">
+      <c r="O31" t="n">
         <v>86.6</v>
       </c>
-      <c r="O31" t="n">
+      <c r="P31" t="n">
         <v>40.45</v>
       </c>
-      <c r="P31" t="n">
+      <c r="Q31" t="n">
         <v>1</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="R31" t="n">
         <v>1.51</v>
       </c>
-      <c r="R31" t="n">
+      <c r="S31" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" t="n">
         <v>2.75</v>
@@ -2327,30 +2423,33 @@
         <v>3.88</v>
       </c>
       <c r="L32" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="M32" t="n">
         <v>7.75</v>
       </c>
-      <c r="M32" t="n">
+      <c r="N32" t="n">
         <v>4.06</v>
       </c>
-      <c r="N32" t="n">
+      <c r="O32" t="n">
         <v>105.62</v>
       </c>
-      <c r="O32" t="n">
+      <c r="P32" t="n">
         <v>56.67</v>
       </c>
-      <c r="P32" t="n">
+      <c r="Q32" t="n">
         <v>1.88</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="R32" t="n">
         <v>3.04</v>
       </c>
-      <c r="R32" t="n">
+      <c r="S32" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" t="n">
         <v>2.2</v>
@@ -2383,30 +2482,33 @@
         <v>2.4</v>
       </c>
       <c r="L33" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="M33" t="n">
         <v>9.7</v>
       </c>
-      <c r="M33" t="n">
+      <c r="N33" t="n">
         <v>6.22</v>
       </c>
-      <c r="N33" t="n">
+      <c r="O33" t="n">
         <v>99.5</v>
       </c>
-      <c r="O33" t="n">
+      <c r="P33" t="n">
         <v>45.63</v>
       </c>
-      <c r="P33" t="n">
+      <c r="Q33" t="n">
         <v>0.7</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="R33" t="n">
         <v>1.34</v>
       </c>
-      <c r="R33" t="n">
+      <c r="S33" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" t="n">
         <v>0.6</v>
@@ -2439,30 +2541,33 @@
         <v>3.4</v>
       </c>
       <c r="L34" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="M34" t="n">
         <v>7.07</v>
       </c>
-      <c r="M34" t="n">
+      <c r="N34" t="n">
         <v>3.99</v>
       </c>
-      <c r="N34" t="n">
+      <c r="O34" t="n">
         <v>87.93</v>
       </c>
-      <c r="O34" t="n">
+      <c r="P34" t="n">
         <v>43.97</v>
       </c>
-      <c r="P34" t="n">
+      <c r="Q34" t="n">
         <v>1</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="R34" t="n">
         <v>1.41</v>
       </c>
-      <c r="R34" t="n">
+      <c r="S34" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" t="n">
         <v>2.45</v>
@@ -2495,30 +2600,33 @@
         <v>3.55</v>
       </c>
       <c r="L35" t="n">
+        <v>1.86</v>
+      </c>
+      <c r="M35" t="n">
         <v>5.91</v>
       </c>
-      <c r="M35" t="n">
+      <c r="N35" t="n">
         <v>4.3</v>
       </c>
-      <c r="N35" t="n">
+      <c r="O35" t="n">
         <v>77.18</v>
       </c>
-      <c r="O35" t="n">
+      <c r="P35" t="n">
         <v>41.66</v>
       </c>
-      <c r="P35" t="n">
+      <c r="Q35" t="n">
         <v>0.27</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="R35" t="n">
         <v>0.65</v>
       </c>
-      <c r="R35" t="n">
+      <c r="S35" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B36" t="n">
         <v>1.57</v>
@@ -2551,30 +2659,33 @@
         <v>3.57</v>
       </c>
       <c r="L36" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="M36" t="n">
         <v>10.57</v>
       </c>
-      <c r="M36" t="n">
+      <c r="N36" t="n">
         <v>7.41</v>
       </c>
-      <c r="N36" t="n">
+      <c r="O36" t="n">
         <v>119.29</v>
       </c>
-      <c r="O36" t="n">
+      <c r="P36" t="n">
         <v>72.73</v>
       </c>
-      <c r="P36" t="n">
+      <c r="Q36" t="n">
         <v>1.71</v>
       </c>
-      <c r="Q36" t="n">
+      <c r="R36" t="n">
         <v>1.5</v>
       </c>
-      <c r="R36" t="n">
+      <c r="S36" t="n">
         <v>7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" t="n">
         <v>1.89</v>
@@ -2607,30 +2718,33 @@
         <v>3.33</v>
       </c>
       <c r="L37" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="M37" t="n">
         <v>8.11</v>
       </c>
-      <c r="M37" t="n">
+      <c r="N37" t="n">
         <v>3.82</v>
       </c>
-      <c r="N37" t="n">
+      <c r="O37" t="n">
         <v>87.78</v>
       </c>
-      <c r="O37" t="n">
+      <c r="P37" t="n">
         <v>36.52</v>
       </c>
-      <c r="P37" t="n">
+      <c r="Q37" t="n">
         <v>1.11</v>
       </c>
-      <c r="Q37" t="n">
+      <c r="R37" t="n">
         <v>1.05</v>
       </c>
-      <c r="R37" t="n">
+      <c r="S37" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B38" t="n">
         <v>0.25</v>
@@ -2663,30 +2777,33 @@
         <v>2</v>
       </c>
       <c r="L38" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="M38" t="n">
         <v>7.75</v>
       </c>
-      <c r="M38" t="n">
+      <c r="N38" t="n">
         <v>5.99</v>
       </c>
-      <c r="N38" t="n">
+      <c r="O38" t="n">
         <v>93</v>
       </c>
-      <c r="O38" t="n">
+      <c r="P38" t="n">
         <v>43.59</v>
       </c>
-      <c r="P38" t="n">
+      <c r="Q38" t="n">
         <v>0.38</v>
       </c>
-      <c r="Q38" t="n">
+      <c r="R38" t="n">
         <v>0.52</v>
       </c>
-      <c r="R38" t="n">
+      <c r="S38" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B39" t="n">
         <v>1.36</v>
@@ -2719,30 +2836,33 @@
         <v>4.64</v>
       </c>
       <c r="L39" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="M39" t="n">
         <v>6</v>
       </c>
-      <c r="M39" t="n">
+      <c r="N39" t="n">
         <v>2.61</v>
       </c>
-      <c r="N39" t="n">
+      <c r="O39" t="n">
         <v>65.82</v>
       </c>
-      <c r="O39" t="n">
+      <c r="P39" t="n">
         <v>26.26</v>
       </c>
-      <c r="P39" t="n">
+      <c r="Q39" t="n">
         <v>0.45</v>
       </c>
-      <c r="Q39" t="n">
+      <c r="R39" t="n">
         <v>0.69</v>
       </c>
-      <c r="R39" t="n">
+      <c r="S39" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B40" t="n">
         <v>2.38</v>
@@ -2775,30 +2895,33 @@
         <v>4</v>
       </c>
       <c r="L40" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M40" t="n">
         <v>5.12</v>
       </c>
-      <c r="M40" t="n">
+      <c r="N40" t="n">
         <v>2.53</v>
       </c>
-      <c r="N40" t="n">
+      <c r="O40" t="n">
         <v>70.12</v>
       </c>
-      <c r="O40" t="n">
+      <c r="P40" t="n">
         <v>31.53</v>
       </c>
-      <c r="P40" t="n">
+      <c r="Q40" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q40" t="n">
+      <c r="R40" t="n">
         <v>0.76</v>
       </c>
-      <c r="R40" t="n">
+      <c r="S40" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B41" t="n">
         <v>0.8</v>
@@ -2831,30 +2954,33 @@
         <v>2.47</v>
       </c>
       <c r="L41" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="M41" t="n">
         <v>5.6</v>
       </c>
-      <c r="M41" t="n">
+      <c r="N41" t="n">
         <v>3.25</v>
       </c>
-      <c r="N41" t="n">
+      <c r="O41" t="n">
         <v>69.13</v>
       </c>
-      <c r="O41" t="n">
+      <c r="P41" t="n">
         <v>35.65</v>
       </c>
-      <c r="P41" t="n">
+      <c r="Q41" t="n">
         <v>0.07</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="R41" t="n">
         <v>0.26</v>
       </c>
-      <c r="R41" t="n">
+      <c r="S41" t="n">
         <v>15</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B42" t="n">
         <v>0.89</v>
@@ -2887,30 +3013,33 @@
         <v>3.89</v>
       </c>
       <c r="L42" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="M42" t="n">
         <v>7.11</v>
       </c>
-      <c r="M42" t="n">
+      <c r="N42" t="n">
         <v>3.37</v>
       </c>
-      <c r="N42" t="n">
+      <c r="O42" t="n">
         <v>73.33</v>
       </c>
-      <c r="O42" t="n">
+      <c r="P42" t="n">
         <v>30.45</v>
       </c>
-      <c r="P42" t="n">
+      <c r="Q42" t="n">
         <v>0.67</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="R42" t="n">
         <v>1.32</v>
       </c>
-      <c r="R42" t="n">
+      <c r="S42" t="n">
         <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B43" t="n">
         <v>0.77</v>
@@ -2943,30 +3072,33 @@
         <v>4.7</v>
       </c>
       <c r="L43" t="n">
+        <v>2.31</v>
+      </c>
+      <c r="M43" t="n">
         <v>6.35</v>
       </c>
-      <c r="M43" t="n">
+      <c r="N43" t="n">
         <v>2.68</v>
       </c>
-      <c r="N43" t="n">
+      <c r="O43" t="n">
         <v>83.67</v>
       </c>
-      <c r="O43" t="n">
+      <c r="P43" t="n">
         <v>32.94</v>
       </c>
-      <c r="P43" t="n">
+      <c r="Q43" t="n">
         <v>0.4</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="R43" t="n">
         <v>0.7</v>
       </c>
-      <c r="R43" t="n">
+      <c r="S43" t="n">
         <v>198</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B44" t="n">
         <v>0.35</v>
@@ -2999,30 +3131,33 @@
         <v>2.41</v>
       </c>
       <c r="L44" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="M44" t="n">
         <v>5.1</v>
       </c>
-      <c r="M44" t="n">
+      <c r="N44" t="n">
         <v>2.44</v>
       </c>
-      <c r="N44" t="n">
+      <c r="O44" t="n">
         <v>58.99</v>
       </c>
-      <c r="O44" t="n">
+      <c r="P44" t="n">
         <v>25.32</v>
       </c>
-      <c r="P44" t="n">
+      <c r="Q44" t="n">
         <v>0.5</v>
       </c>
-      <c r="Q44" t="n">
+      <c r="R44" t="n">
         <v>0.73</v>
       </c>
-      <c r="R44" t="n">
+      <c r="S44" t="n">
         <v>354</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B45" t="n">
         <v>2.39</v>
@@ -3055,30 +3190,33 @@
         <v>3.61</v>
       </c>
       <c r="L45" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="M45" t="n">
         <v>6.96</v>
       </c>
-      <c r="M45" t="n">
+      <c r="N45" t="n">
         <v>3.25</v>
       </c>
-      <c r="N45" t="n">
+      <c r="O45" t="n">
         <v>92.56</v>
       </c>
-      <c r="O45" t="n">
+      <c r="P45" t="n">
         <v>37.2</v>
       </c>
-      <c r="P45" t="n">
+      <c r="Q45" t="n">
         <v>0.57</v>
       </c>
-      <c r="Q45" t="n">
+      <c r="R45" t="n">
         <v>0.96</v>
       </c>
-      <c r="R45" t="n">
+      <c r="S45" t="n">
         <v>2311</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B46" t="n">
         <v>0.47</v>
@@ -3111,30 +3249,33 @@
         <v>2.23</v>
       </c>
       <c r="L46" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="M46" t="n">
         <v>6.57</v>
       </c>
-      <c r="M46" t="n">
+      <c r="N46" t="n">
         <v>3.16</v>
       </c>
-      <c r="N46" t="n">
+      <c r="O46" t="n">
         <v>93.7</v>
       </c>
-      <c r="O46" t="n">
+      <c r="P46" t="n">
         <v>35.73</v>
       </c>
-      <c r="P46" t="n">
+      <c r="Q46" t="n">
         <v>0.78</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="R46" t="n">
         <v>1.12</v>
       </c>
-      <c r="R46" t="n">
+      <c r="S46" t="n">
         <v>2612</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B47" t="n">
         <v>0.13</v>
@@ -3167,30 +3308,33 @@
         <v>3.7</v>
       </c>
       <c r="L47" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M47" t="n">
         <v>7.72</v>
       </c>
-      <c r="M47" t="n">
+      <c r="N47" t="n">
         <v>3.24</v>
       </c>
-      <c r="N47" t="n">
+      <c r="O47" t="n">
         <v>86.26</v>
       </c>
-      <c r="O47" t="n">
+      <c r="P47" t="n">
         <v>29.43</v>
       </c>
-      <c r="P47" t="n">
+      <c r="Q47" t="n">
         <v>0.66</v>
       </c>
-      <c r="Q47" t="n">
+      <c r="R47" t="n">
         <v>0.89</v>
       </c>
-      <c r="R47" t="n">
+      <c r="S47" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B48" t="n">
         <v>2.48</v>
@@ -3223,30 +3367,33 @@
         <v>4.28</v>
       </c>
       <c r="L48" t="n">
+        <v>3</v>
+      </c>
+      <c r="M48" t="n">
         <v>7.55</v>
       </c>
-      <c r="M48" t="n">
+      <c r="N48" t="n">
         <v>3.37</v>
       </c>
-      <c r="N48" t="n">
+      <c r="O48" t="n">
         <v>89.74</v>
       </c>
-      <c r="O48" t="n">
+      <c r="P48" t="n">
         <v>32.9</v>
       </c>
-      <c r="P48" t="n">
+      <c r="Q48" t="n">
         <v>1.18</v>
       </c>
-      <c r="Q48" t="n">
+      <c r="R48" t="n">
         <v>1.17</v>
       </c>
-      <c r="R48" t="n">
+      <c r="S48" t="n">
         <v>141</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B49" t="n">
         <v>3.26</v>
@@ -3279,30 +3426,33 @@
         <v>3.98</v>
       </c>
       <c r="L49" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="M49" t="n">
         <v>7.09</v>
       </c>
-      <c r="M49" t="n">
+      <c r="N49" t="n">
         <v>2.75</v>
       </c>
-      <c r="N49" t="n">
+      <c r="O49" t="n">
         <v>96.16</v>
       </c>
-      <c r="O49" t="n">
+      <c r="P49" t="n">
         <v>27.67</v>
       </c>
-      <c r="P49" t="n">
+      <c r="Q49" t="n">
         <v>0.89</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="R49" t="n">
         <v>0.99</v>
       </c>
-      <c r="R49" t="n">
+      <c r="S49" t="n">
         <v>81</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B50" t="n">
         <v>0.73</v>
@@ -3335,30 +3485,33 @@
         <v>2.72</v>
       </c>
       <c r="L50" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="M50" t="n">
         <v>7.08</v>
       </c>
-      <c r="M50" t="n">
+      <c r="N50" t="n">
         <v>3.4</v>
       </c>
-      <c r="N50" t="n">
+      <c r="O50" t="n">
         <v>90.73</v>
       </c>
-      <c r="O50" t="n">
+      <c r="P50" t="n">
         <v>36.98</v>
       </c>
-      <c r="P50" t="n">
+      <c r="Q50" t="n">
         <v>0.52</v>
       </c>
-      <c r="Q50" t="n">
+      <c r="R50" t="n">
         <v>0.87</v>
       </c>
-      <c r="R50" t="n">
+      <c r="S50" t="n">
         <v>2316</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B51" t="n">
         <v>0.98</v>
@@ -3391,30 +3544,33 @@
         <v>2.79</v>
       </c>
       <c r="L51" t="n">
+        <v>2.14</v>
+      </c>
+      <c r="M51" t="n">
         <v>7.16</v>
       </c>
-      <c r="M51" t="n">
+      <c r="N51" t="n">
         <v>3.92</v>
       </c>
-      <c r="N51" t="n">
+      <c r="O51" t="n">
         <v>99.18</v>
       </c>
-      <c r="O51" t="n">
+      <c r="P51" t="n">
         <v>46.33</v>
       </c>
-      <c r="P51" t="n">
+      <c r="Q51" t="n">
         <v>1.01</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="R51" t="n">
         <v>1.29</v>
       </c>
-      <c r="R51" t="n">
+      <c r="S51" t="n">
         <v>143</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B52" t="n">
         <v>0.94</v>
@@ -3447,30 +3603,33 @@
         <v>1.78</v>
       </c>
       <c r="L52" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="M52" t="n">
         <v>7.44</v>
       </c>
-      <c r="M52" t="n">
+      <c r="N52" t="n">
         <v>4.95</v>
       </c>
-      <c r="N52" t="n">
+      <c r="O52" t="n">
         <v>89.66</v>
       </c>
-      <c r="O52" t="n">
+      <c r="P52" t="n">
         <v>42.77</v>
       </c>
-      <c r="P52" t="n">
+      <c r="Q52" t="n">
         <v>0.93</v>
       </c>
-      <c r="Q52" t="n">
+      <c r="R52" t="n">
         <v>1.05</v>
       </c>
-      <c r="R52" t="n">
+      <c r="S52" t="n">
         <v>123</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B53" t="n">
         <v>1.56</v>
@@ -3503,30 +3662,33 @@
         <v>3.44</v>
       </c>
       <c r="L53" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="M53" t="n">
         <v>7.03</v>
       </c>
-      <c r="M53" t="n">
+      <c r="N53" t="n">
         <v>3.86</v>
       </c>
-      <c r="N53" t="n">
+      <c r="O53" t="n">
         <v>94.18</v>
       </c>
-      <c r="O53" t="n">
+      <c r="P53" t="n">
         <v>40.32</v>
       </c>
-      <c r="P53" t="n">
+      <c r="Q53" t="n">
         <v>0.91</v>
       </c>
-      <c r="Q53" t="n">
+      <c r="R53" t="n">
         <v>1.19</v>
       </c>
-      <c r="R53" t="n">
+      <c r="S53" t="n">
         <v>119</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B54" t="n">
         <v>0.34</v>
@@ -3559,24 +3721,27 @@
         <v>3.13</v>
       </c>
       <c r="L54" t="n">
+        <v>2.04</v>
+      </c>
+      <c r="M54" t="n">
         <v>6.68</v>
       </c>
-      <c r="M54" t="n">
+      <c r="N54" t="n">
         <v>3.06</v>
       </c>
-      <c r="N54" t="n">
+      <c r="O54" t="n">
         <v>90.68</v>
       </c>
-      <c r="O54" t="n">
+      <c r="P54" t="n">
         <v>34.38</v>
       </c>
-      <c r="P54" t="n">
+      <c r="Q54" t="n">
         <v>0.69</v>
       </c>
-      <c r="Q54" t="n">
+      <c r="R54" t="n">
         <v>1.02</v>
       </c>
-      <c r="R54" t="n">
+      <c r="S54" t="n">
         <v>2331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Close to submission of revision
</commit_message>
<xml_diff>
--- a/R/processed_data/picturePulls.xlsx
+++ b/R/processed_data/picturePulls.xlsx
@@ -727,10 +727,10 @@
         <v>35.27</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.38</v>
+        <v>0.42</v>
       </c>
       <c r="R3" t="n">
-        <v>0.8</v>
+        <v>0.86</v>
       </c>
       <c r="S3" t="n">
         <v>408</v>
@@ -786,10 +786,10 @@
         <v>34.25</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
       <c r="R4" t="n">
-        <v>0.96</v>
+        <v>0.97</v>
       </c>
       <c r="S4" t="n">
         <v>797</v>
@@ -845,10 +845,10 @@
         <v>62.22</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.11</v>
+        <v>0.95</v>
       </c>
       <c r="R5" t="n">
-        <v>1.46</v>
+        <v>1.41</v>
       </c>
       <c r="S5" t="n">
         <v>83</v>
@@ -963,10 +963,10 @@
         <v>30.97</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.98</v>
+        <v>0.89</v>
       </c>
       <c r="R7" t="n">
-        <v>1.31</v>
+        <v>1.22</v>
       </c>
       <c r="S7" t="n">
         <v>141</v>
@@ -1022,10 +1022,10 @@
         <v>43.68</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.59</v>
+        <v>0.47</v>
       </c>
       <c r="R8" t="n">
-        <v>0.9</v>
+        <v>0.74</v>
       </c>
       <c r="S8" t="n">
         <v>111</v>
@@ -1084,7 +1084,7 @@
         <v>0.72</v>
       </c>
       <c r="R9" t="n">
-        <v>1.11</v>
+        <v>1.1</v>
       </c>
       <c r="S9" t="n">
         <v>1854</v>
@@ -1140,10 +1140,10 @@
         <v>40.26</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.79</v>
+        <v>0.78</v>
       </c>
       <c r="R10" t="n">
-        <v>1.08</v>
+        <v>1</v>
       </c>
       <c r="S10" t="n">
         <v>125</v>
@@ -1202,7 +1202,7 @@
         <v>0.44</v>
       </c>
       <c r="R11" t="n">
-        <v>0.74</v>
+        <v>0.75</v>
       </c>
       <c r="S11" t="n">
         <v>799</v>
@@ -1258,10 +1258,10 @@
         <v>36</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.73</v>
+        <v>0.68</v>
       </c>
       <c r="R12" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="S12" t="n">
         <v>97</v>
@@ -1317,10 +1317,10 @@
         <v>27.11</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.36</v>
+        <v>0.38</v>
       </c>
       <c r="R13" t="n">
-        <v>0.73</v>
+        <v>0.76</v>
       </c>
       <c r="S13" t="n">
         <v>95</v>
@@ -1376,10 +1376,10 @@
         <v>35.08</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.98</v>
+        <v>0.97</v>
       </c>
       <c r="R14" t="n">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="S14" t="n">
         <v>202</v>
@@ -1435,10 +1435,10 @@
         <v>34.91</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.35</v>
+        <v>0.38</v>
       </c>
       <c r="R15" t="n">
-        <v>0.59</v>
+        <v>0.65</v>
       </c>
       <c r="S15" t="n">
         <v>196</v>
@@ -1553,10 +1553,10 @@
         <v>33.61</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.65</v>
+        <v>0.68</v>
       </c>
       <c r="R17" t="n">
-        <v>0.95</v>
+        <v>0.97</v>
       </c>
       <c r="S17" t="n">
         <v>196</v>
@@ -2025,10 +2025,10 @@
         <v>34.44</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.42</v>
+        <v>0.39</v>
       </c>
       <c r="R25" t="n">
-        <v>0.74</v>
+        <v>0.69</v>
       </c>
       <c r="S25" t="n">
         <v>200</v>
@@ -3087,10 +3087,10 @@
         <v>32.94</v>
       </c>
       <c r="Q43" t="n">
-        <v>0.4</v>
+        <v>0.37</v>
       </c>
       <c r="R43" t="n">
-        <v>0.7</v>
+        <v>0.66</v>
       </c>
       <c r="S43" t="n">
         <v>198</v>
@@ -3146,10 +3146,10 @@
         <v>25.32</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.5</v>
+        <v>0.47</v>
       </c>
       <c r="R44" t="n">
-        <v>0.73</v>
+        <v>0.71</v>
       </c>
       <c r="S44" t="n">
         <v>354</v>
@@ -3264,10 +3264,10 @@
         <v>35.73</v>
       </c>
       <c r="Q46" t="n">
-        <v>0.78</v>
+        <v>0.77</v>
       </c>
       <c r="R46" t="n">
-        <v>1.12</v>
+        <v>1.11</v>
       </c>
       <c r="S46" t="n">
         <v>2612</v>
@@ -3323,10 +3323,10 @@
         <v>29.43</v>
       </c>
       <c r="Q47" t="n">
-        <v>0.66</v>
+        <v>0.67</v>
       </c>
       <c r="R47" t="n">
-        <v>0.89</v>
+        <v>0.87</v>
       </c>
       <c r="S47" t="n">
         <v>141</v>
@@ -3382,10 +3382,10 @@
         <v>32.9</v>
       </c>
       <c r="Q48" t="n">
-        <v>1.18</v>
+        <v>1.06</v>
       </c>
       <c r="R48" t="n">
-        <v>1.17</v>
+        <v>1.13</v>
       </c>
       <c r="S48" t="n">
         <v>141</v>
@@ -3441,10 +3441,10 @@
         <v>27.67</v>
       </c>
       <c r="Q49" t="n">
-        <v>0.89</v>
+        <v>0.83</v>
       </c>
       <c r="R49" t="n">
-        <v>0.99</v>
+        <v>0.96</v>
       </c>
       <c r="S49" t="n">
         <v>81</v>
@@ -3500,7 +3500,7 @@
         <v>36.98</v>
       </c>
       <c r="Q50" t="n">
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="R50" t="n">
         <v>0.87</v>
@@ -3559,10 +3559,10 @@
         <v>46.33</v>
       </c>
       <c r="Q51" t="n">
-        <v>1.01</v>
+        <v>1.05</v>
       </c>
       <c r="R51" t="n">
-        <v>1.29</v>
+        <v>1.34</v>
       </c>
       <c r="S51" t="n">
         <v>143</v>
@@ -3618,10 +3618,10 @@
         <v>42.77</v>
       </c>
       <c r="Q52" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="R52" t="n">
         <v>0.93</v>
-      </c>
-      <c r="R52" t="n">
-        <v>1.05</v>
       </c>
       <c r="S52" t="n">
         <v>123</v>
@@ -3677,10 +3677,10 @@
         <v>40.32</v>
       </c>
       <c r="Q53" t="n">
-        <v>0.91</v>
+        <v>0.8</v>
       </c>
       <c r="R53" t="n">
-        <v>1.19</v>
+        <v>1.08</v>
       </c>
       <c r="S53" t="n">
         <v>119</v>
@@ -3739,7 +3739,7 @@
         <v>0.69</v>
       </c>
       <c r="R54" t="n">
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="S54" t="n">
         <v>2331</v>

</xml_diff>

<commit_message>
Final (?) version, except PsychArchives Link
</commit_message>
<xml_diff>
--- a/R/processed_data/picturePulls.xlsx
+++ b/R/processed_data/picturePulls.xlsx
@@ -89,13 +89,16 @@
     <t xml:space="preserve">burglar</t>
   </si>
   <si>
-    <t xml:space="preserve">canyon</t>
+    <t xml:space="preserve">canyon (TAT 11)</t>
   </si>
   <si>
     <t xml:space="preserve">couple by river</t>
   </si>
   <si>
-    <t xml:space="preserve">group</t>
+    <t xml:space="preserve">girlfriends in cafe with male approaching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group (TAT 9BM)</t>
   </si>
   <si>
     <t xml:space="preserve">kennedy nixon</t>
@@ -212,19 +215,16 @@
     <t xml:space="preserve">sorrow</t>
   </si>
   <si>
-    <t xml:space="preserve">three people</t>
-  </si>
-  <si>
     <t xml:space="preserve">trapeze artists</t>
   </si>
   <si>
-    <t xml:space="preserve">violin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">window</t>
-  </si>
-  <si>
-    <t xml:space="preserve">woman</t>
+    <t xml:space="preserve">violin (TAT 1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">window (TAT 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">woman (TAT 9GF)</t>
   </si>
   <si>
     <t xml:space="preserve">women in laboratory</t>
@@ -1095,58 +1095,58 @@
         <v>27</v>
       </c>
       <c r="B10" t="n">
-        <v>0.85</v>
+        <v>3.26</v>
       </c>
       <c r="C10" t="n">
-        <v>1.23</v>
+        <v>1.84</v>
       </c>
       <c r="D10" t="n">
-        <v>0.47</v>
+        <v>0.94</v>
       </c>
       <c r="E10" t="n">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="F10" t="n">
-        <v>0.55</v>
+        <v>0.22</v>
       </c>
       <c r="G10" t="n">
-        <v>0.14</v>
+        <v>0.01</v>
       </c>
       <c r="H10" t="n">
-        <v>1.13</v>
+        <v>0.69</v>
       </c>
       <c r="I10" t="n">
-        <v>1.15</v>
+        <v>1.02</v>
       </c>
       <c r="J10" t="n">
-        <v>0.62</v>
+        <v>0.44</v>
       </c>
       <c r="K10" t="n">
-        <v>2.18</v>
+        <v>3.98</v>
       </c>
       <c r="L10" t="n">
-        <v>1.85</v>
+        <v>1.99</v>
       </c>
       <c r="M10" t="n">
-        <v>6.88</v>
+        <v>7.09</v>
       </c>
       <c r="N10" t="n">
-        <v>3.88</v>
+        <v>2.75</v>
       </c>
       <c r="O10" t="n">
-        <v>88.97</v>
+        <v>96.16</v>
       </c>
       <c r="P10" t="n">
-        <v>40.26</v>
+        <v>27.67</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.8</v>
+        <v>0.86</v>
       </c>
       <c r="R10" t="n">
-        <v>1.12</v>
+        <v>0.98</v>
       </c>
       <c r="S10" t="n">
-        <v>125</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11">
@@ -1154,58 +1154,58 @@
         <v>28</v>
       </c>
       <c r="B11" t="n">
-        <v>0.1</v>
+        <v>0.85</v>
       </c>
       <c r="C11" t="n">
-        <v>0.38</v>
+        <v>1.23</v>
       </c>
       <c r="D11" t="n">
-        <v>0.08</v>
+        <v>0.47</v>
       </c>
       <c r="E11" t="n">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
       <c r="F11" t="n">
-        <v>1.33</v>
+        <v>0.55</v>
       </c>
       <c r="G11" t="n">
-        <v>0.64</v>
+        <v>0.14</v>
       </c>
       <c r="H11" t="n">
-        <v>1.82</v>
+        <v>1.13</v>
       </c>
       <c r="I11" t="n">
-        <v>1.43</v>
+        <v>1.15</v>
       </c>
       <c r="J11" t="n">
-        <v>0.83</v>
+        <v>0.62</v>
       </c>
       <c r="K11" t="n">
-        <v>3.22</v>
+        <v>2.18</v>
       </c>
       <c r="L11" t="n">
-        <v>1.99</v>
+        <v>1.85</v>
       </c>
       <c r="M11" t="n">
-        <v>5.94</v>
+        <v>6.88</v>
       </c>
       <c r="N11" t="n">
-        <v>2.67</v>
+        <v>3.88</v>
       </c>
       <c r="O11" t="n">
-        <v>84.96</v>
+        <v>88.97</v>
       </c>
       <c r="P11" t="n">
-        <v>31.05</v>
+        <v>40.26</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.45</v>
+        <v>0.8</v>
       </c>
       <c r="R11" t="n">
-        <v>0.75</v>
+        <v>1.12</v>
       </c>
       <c r="S11" t="n">
-        <v>799</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12">
@@ -1213,58 +1213,58 @@
         <v>29</v>
       </c>
       <c r="B12" t="n">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C12" t="n">
-        <v>0.47</v>
+        <v>0.38</v>
       </c>
       <c r="D12" t="n">
-        <v>0.16</v>
+        <v>0.08</v>
       </c>
       <c r="E12" t="n">
-        <v>1.95</v>
+        <v>1.3</v>
       </c>
       <c r="F12" t="n">
-        <v>1.36</v>
+        <v>1.33</v>
       </c>
       <c r="G12" t="n">
-        <v>0.87</v>
+        <v>0.64</v>
       </c>
       <c r="H12" t="n">
-        <v>0.3</v>
+        <v>1.82</v>
       </c>
       <c r="I12" t="n">
-        <v>0.52</v>
+        <v>1.43</v>
       </c>
       <c r="J12" t="n">
-        <v>0.27</v>
+        <v>0.83</v>
       </c>
       <c r="K12" t="n">
-        <v>2.44</v>
+        <v>3.22</v>
       </c>
       <c r="L12" t="n">
-        <v>1.41</v>
+        <v>1.99</v>
       </c>
       <c r="M12" t="n">
-        <v>6.86</v>
+        <v>5.94</v>
       </c>
       <c r="N12" t="n">
-        <v>3.12</v>
+        <v>2.67</v>
       </c>
       <c r="O12" t="n">
-        <v>92.34</v>
+        <v>84.96</v>
       </c>
       <c r="P12" t="n">
-        <v>36</v>
+        <v>31.05</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.68</v>
+        <v>0.44</v>
       </c>
       <c r="R12" t="n">
-        <v>0.97</v>
+        <v>0.75</v>
       </c>
       <c r="S12" t="n">
-        <v>97</v>
+        <v>799</v>
       </c>
     </row>
     <row r="13">
@@ -1272,58 +1272,58 @@
         <v>30</v>
       </c>
       <c r="B13" t="n">
-        <v>0.08</v>
+        <v>0.2</v>
       </c>
       <c r="C13" t="n">
-        <v>0.35</v>
+        <v>0.47</v>
       </c>
       <c r="D13" t="n">
-        <v>0.06</v>
+        <v>0.16</v>
       </c>
       <c r="E13" t="n">
-        <v>0.31</v>
+        <v>1.95</v>
       </c>
       <c r="F13" t="n">
-        <v>0.62</v>
+        <v>1.36</v>
       </c>
       <c r="G13" t="n">
-        <v>0.25</v>
+        <v>0.87</v>
       </c>
       <c r="H13" t="n">
-        <v>0.79</v>
+        <v>0.3</v>
       </c>
       <c r="I13" t="n">
-        <v>0.78</v>
+        <v>0.52</v>
       </c>
       <c r="J13" t="n">
-        <v>0.59</v>
+        <v>0.27</v>
       </c>
       <c r="K13" t="n">
-        <v>1.18</v>
+        <v>2.44</v>
       </c>
       <c r="L13" t="n">
-        <v>1.1</v>
+        <v>1.41</v>
       </c>
       <c r="M13" t="n">
-        <v>5.98</v>
+        <v>6.86</v>
       </c>
       <c r="N13" t="n">
-        <v>2.71</v>
+        <v>3.12</v>
       </c>
       <c r="O13" t="n">
-        <v>86.08</v>
+        <v>92.34</v>
       </c>
       <c r="P13" t="n">
-        <v>27.11</v>
+        <v>36</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.37</v>
+        <v>0.68</v>
       </c>
       <c r="R13" t="n">
-        <v>0.76</v>
+        <v>0.97</v>
       </c>
       <c r="S13" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14">
@@ -1331,58 +1331,58 @@
         <v>31</v>
       </c>
       <c r="B14" t="n">
-        <v>0.49</v>
+        <v>0.08</v>
       </c>
       <c r="C14" t="n">
-        <v>0.84</v>
+        <v>0.35</v>
       </c>
       <c r="D14" t="n">
-        <v>0.34</v>
+        <v>0.06</v>
       </c>
       <c r="E14" t="n">
-        <v>0.85</v>
+        <v>0.31</v>
       </c>
       <c r="F14" t="n">
-        <v>1.09</v>
+        <v>0.62</v>
       </c>
       <c r="G14" t="n">
-        <v>0.52</v>
+        <v>0.25</v>
       </c>
       <c r="H14" t="n">
-        <v>0.82</v>
+        <v>0.79</v>
       </c>
       <c r="I14" t="n">
-        <v>1.03</v>
+        <v>0.78</v>
       </c>
       <c r="J14" t="n">
-        <v>0.5</v>
+        <v>0.59</v>
       </c>
       <c r="K14" t="n">
-        <v>2.16</v>
+        <v>1.18</v>
       </c>
       <c r="L14" t="n">
-        <v>1.75</v>
+        <v>1.1</v>
       </c>
       <c r="M14" t="n">
-        <v>6</v>
+        <v>5.98</v>
       </c>
       <c r="N14" t="n">
-        <v>2.5</v>
+        <v>2.71</v>
       </c>
       <c r="O14" t="n">
-        <v>82.48</v>
+        <v>86.08</v>
       </c>
       <c r="P14" t="n">
-        <v>35.08</v>
+        <v>27.11</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.97</v>
+        <v>0.37</v>
       </c>
       <c r="R14" t="n">
-        <v>1.2</v>
+        <v>0.76</v>
       </c>
       <c r="S14" t="n">
-        <v>202</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15">
@@ -1390,58 +1390,58 @@
         <v>32</v>
       </c>
       <c r="B15" t="n">
-        <v>1.71</v>
+        <v>0.49</v>
       </c>
       <c r="C15" t="n">
-        <v>1.22</v>
+        <v>0.84</v>
       </c>
       <c r="D15" t="n">
-        <v>0.86</v>
+        <v>0.34</v>
       </c>
       <c r="E15" t="n">
-        <v>0.68</v>
+        <v>0.85</v>
       </c>
       <c r="F15" t="n">
-        <v>1.08</v>
+        <v>1.09</v>
       </c>
       <c r="G15" t="n">
-        <v>0.44</v>
+        <v>0.52</v>
       </c>
       <c r="H15" t="n">
-        <v>0.92</v>
+        <v>0.82</v>
       </c>
       <c r="I15" t="n">
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="J15" t="n">
-        <v>0.56</v>
+        <v>0.5</v>
       </c>
       <c r="K15" t="n">
-        <v>3.32</v>
+        <v>2.16</v>
       </c>
       <c r="L15" t="n">
-        <v>1.92</v>
+        <v>1.75</v>
       </c>
       <c r="M15" t="n">
-        <v>6.54</v>
+        <v>6</v>
       </c>
       <c r="N15" t="n">
-        <v>2.7</v>
+        <v>2.5</v>
       </c>
       <c r="O15" t="n">
-        <v>86.97</v>
+        <v>82.48</v>
       </c>
       <c r="P15" t="n">
-        <v>34.91</v>
+        <v>35.08</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.38</v>
+        <v>0.97</v>
       </c>
       <c r="R15" t="n">
-        <v>0.65</v>
+        <v>1.2</v>
       </c>
       <c r="S15" t="n">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="16">
@@ -1449,58 +1449,58 @@
         <v>33</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4</v>
+        <v>1.71</v>
       </c>
       <c r="C16" t="n">
-        <v>0.7</v>
+        <v>1.22</v>
       </c>
       <c r="D16" t="n">
-        <v>0.3</v>
+        <v>0.86</v>
       </c>
       <c r="E16" t="n">
-        <v>0.1</v>
+        <v>0.68</v>
       </c>
       <c r="F16" t="n">
-        <v>0.32</v>
+        <v>1.08</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1</v>
+        <v>0.44</v>
       </c>
       <c r="H16" t="n">
-        <v>2.3</v>
+        <v>0.92</v>
       </c>
       <c r="I16" t="n">
-        <v>1.57</v>
+        <v>1.05</v>
       </c>
       <c r="J16" t="n">
-        <v>0.8</v>
+        <v>0.56</v>
       </c>
       <c r="K16" t="n">
-        <v>2.8</v>
+        <v>3.32</v>
       </c>
       <c r="L16" t="n">
-        <v>1.75</v>
+        <v>1.92</v>
       </c>
       <c r="M16" t="n">
-        <v>6.8</v>
+        <v>6.54</v>
       </c>
       <c r="N16" t="n">
-        <v>3.91</v>
+        <v>2.7</v>
       </c>
       <c r="O16" t="n">
-        <v>87.1</v>
+        <v>86.97</v>
       </c>
       <c r="P16" t="n">
-        <v>51.74</v>
+        <v>34.91</v>
       </c>
       <c r="Q16" t="n">
-        <v>1.2</v>
+        <v>0.38</v>
       </c>
       <c r="R16" t="n">
-        <v>1.4</v>
+        <v>0.65</v>
       </c>
       <c r="S16" t="n">
-        <v>10</v>
+        <v>196</v>
       </c>
     </row>
     <row r="17">
@@ -1508,58 +1508,58 @@
         <v>34</v>
       </c>
       <c r="B17" t="n">
-        <v>0.55</v>
+        <v>0.4</v>
       </c>
       <c r="C17" t="n">
-        <v>0.94</v>
+        <v>0.7</v>
       </c>
       <c r="D17" t="n">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="E17" t="n">
-        <v>0.82</v>
+        <v>0.1</v>
       </c>
       <c r="F17" t="n">
-        <v>1.11</v>
+        <v>0.32</v>
       </c>
       <c r="G17" t="n">
-        <v>0.47</v>
+        <v>0.1</v>
       </c>
       <c r="H17" t="n">
-        <v>1.27</v>
+        <v>2.3</v>
       </c>
       <c r="I17" t="n">
-        <v>1.51</v>
+        <v>1.57</v>
       </c>
       <c r="J17" t="n">
-        <v>0.63</v>
+        <v>0.8</v>
       </c>
       <c r="K17" t="n">
-        <v>2.63</v>
+        <v>2.8</v>
       </c>
       <c r="L17" t="n">
-        <v>2.41</v>
+        <v>1.75</v>
       </c>
       <c r="M17" t="n">
-        <v>6.33</v>
+        <v>6.8</v>
       </c>
       <c r="N17" t="n">
-        <v>2.83</v>
+        <v>3.91</v>
       </c>
       <c r="O17" t="n">
-        <v>82.91</v>
+        <v>87.1</v>
       </c>
       <c r="P17" t="n">
-        <v>33.61</v>
+        <v>51.74</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.69</v>
+        <v>1.2</v>
       </c>
       <c r="R17" t="n">
-        <v>0.98</v>
+        <v>1.4</v>
       </c>
       <c r="S17" t="n">
-        <v>196</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -1567,58 +1567,58 @@
         <v>35</v>
       </c>
       <c r="B18" t="n">
-        <v>1.18</v>
+        <v>0.55</v>
       </c>
       <c r="C18" t="n">
-        <v>1.4</v>
+        <v>0.94</v>
       </c>
       <c r="D18" t="n">
-        <v>0.55</v>
+        <v>0.35</v>
       </c>
       <c r="E18" t="n">
-        <v>0.18</v>
+        <v>0.82</v>
       </c>
       <c r="F18" t="n">
-        <v>0.4</v>
+        <v>1.11</v>
       </c>
       <c r="G18" t="n">
-        <v>0.18</v>
+        <v>0.47</v>
       </c>
       <c r="H18" t="n">
-        <v>0.82</v>
+        <v>1.27</v>
       </c>
       <c r="I18" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2.63</v>
+      </c>
+      <c r="L18" t="n">
+        <v>2.41</v>
+      </c>
+      <c r="M18" t="n">
+        <v>6.33</v>
+      </c>
+      <c r="N18" t="n">
+        <v>2.83</v>
+      </c>
+      <c r="O18" t="n">
+        <v>82.91</v>
+      </c>
+      <c r="P18" t="n">
+        <v>33.61</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="R18" t="n">
         <v>0.98</v>
       </c>
-      <c r="J18" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="K18" t="n">
-        <v>2.18</v>
-      </c>
-      <c r="L18" t="n">
-        <v>1.17</v>
-      </c>
-      <c r="M18" t="n">
-        <v>6.18</v>
-      </c>
-      <c r="N18" t="n">
-        <v>3.49</v>
-      </c>
-      <c r="O18" t="n">
-        <v>74.73</v>
-      </c>
-      <c r="P18" t="n">
-        <v>32.6</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="R18" t="n">
-        <v>0.69</v>
-      </c>
       <c r="S18" t="n">
-        <v>11</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19">
@@ -1626,58 +1626,58 @@
         <v>36</v>
       </c>
       <c r="B19" t="n">
-        <v>1.88</v>
+        <v>1.18</v>
       </c>
       <c r="C19" t="n">
-        <v>1.13</v>
+        <v>1.4</v>
       </c>
       <c r="D19" t="n">
-        <v>0.88</v>
+        <v>0.55</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="F19" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="H19" t="n">
-        <v>1.38</v>
+        <v>0.82</v>
       </c>
       <c r="I19" t="n">
-        <v>1.3</v>
+        <v>0.98</v>
       </c>
       <c r="J19" t="n">
-        <v>0.62</v>
+        <v>0.55</v>
       </c>
       <c r="K19" t="n">
-        <v>3.25</v>
+        <v>2.18</v>
       </c>
       <c r="L19" t="n">
-        <v>1.75</v>
+        <v>1.17</v>
       </c>
       <c r="M19" t="n">
-        <v>9.75</v>
+        <v>6.18</v>
       </c>
       <c r="N19" t="n">
-        <v>4.2</v>
+        <v>3.49</v>
       </c>
       <c r="O19" t="n">
-        <v>100</v>
+        <v>74.73</v>
       </c>
       <c r="P19" t="n">
-        <v>45.3</v>
+        <v>32.6</v>
       </c>
       <c r="Q19" t="n">
-        <v>1.5</v>
+        <v>0.45</v>
       </c>
       <c r="R19" t="n">
-        <v>0.93</v>
+        <v>0.69</v>
       </c>
       <c r="S19" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20">
@@ -1685,13 +1685,13 @@
         <v>37</v>
       </c>
       <c r="B20" t="n">
-        <v>1.29</v>
+        <v>1.88</v>
       </c>
       <c r="C20" t="n">
-        <v>1.11</v>
+        <v>1.13</v>
       </c>
       <c r="D20" t="n">
-        <v>0.71</v>
+        <v>0.88</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
@@ -1703,40 +1703,40 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>1.43</v>
+        <v>1.38</v>
       </c>
       <c r="I20" t="n">
-        <v>0.79</v>
+        <v>1.3</v>
       </c>
       <c r="J20" t="n">
-        <v>1</v>
+        <v>0.62</v>
       </c>
       <c r="K20" t="n">
-        <v>2.71</v>
+        <v>3.25</v>
       </c>
       <c r="L20" t="n">
-        <v>1.8</v>
+        <v>1.75</v>
       </c>
       <c r="M20" t="n">
-        <v>6.29</v>
+        <v>9.75</v>
       </c>
       <c r="N20" t="n">
-        <v>2.81</v>
+        <v>4.2</v>
       </c>
       <c r="O20" t="n">
-        <v>84.29</v>
+        <v>100</v>
       </c>
       <c r="P20" t="n">
-        <v>30.61</v>
+        <v>45.3</v>
       </c>
       <c r="Q20" t="n">
-        <v>1.43</v>
+        <v>1.5</v>
       </c>
       <c r="R20" t="n">
-        <v>1.51</v>
+        <v>0.93</v>
       </c>
       <c r="S20" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
@@ -1744,58 +1744,58 @@
         <v>38</v>
       </c>
       <c r="B21" t="n">
-        <v>0.09</v>
+        <v>1.29</v>
       </c>
       <c r="C21" t="n">
-        <v>0.3</v>
+        <v>1.11</v>
       </c>
       <c r="D21" t="n">
-        <v>0.09</v>
+        <v>0.71</v>
       </c>
       <c r="E21" t="n">
-        <v>2.55</v>
+        <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>1.81</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>0.91</v>
+        <v>0</v>
       </c>
       <c r="H21" t="n">
-        <v>0.64</v>
+        <v>1.43</v>
       </c>
       <c r="I21" t="n">
-        <v>0.67</v>
+        <v>0.79</v>
       </c>
       <c r="J21" t="n">
-        <v>0.55</v>
+        <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>3.27</v>
+        <v>2.71</v>
       </c>
       <c r="L21" t="n">
-        <v>1.79</v>
+        <v>1.8</v>
       </c>
       <c r="M21" t="n">
-        <v>7.64</v>
+        <v>6.29</v>
       </c>
       <c r="N21" t="n">
-        <v>2.06</v>
+        <v>2.81</v>
       </c>
       <c r="O21" t="n">
-        <v>73.73</v>
+        <v>84.29</v>
       </c>
       <c r="P21" t="n">
-        <v>28.44</v>
+        <v>30.61</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.55</v>
+        <v>1.43</v>
       </c>
       <c r="R21" t="n">
-        <v>0.93</v>
+        <v>1.51</v>
       </c>
       <c r="S21" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -1803,58 +1803,58 @@
         <v>39</v>
       </c>
       <c r="B22" t="n">
-        <v>3.25</v>
+        <v>0.09</v>
       </c>
       <c r="C22" t="n">
-        <v>1.71</v>
+        <v>0.3</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>0.09</v>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>2.55</v>
       </c>
       <c r="F22" t="n">
-        <v>0</v>
+        <v>1.81</v>
       </c>
       <c r="G22" t="n">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="H22" t="n">
-        <v>1.25</v>
+        <v>0.64</v>
       </c>
       <c r="I22" t="n">
-        <v>1.5</v>
+        <v>0.67</v>
       </c>
       <c r="J22" t="n">
-        <v>0.5</v>
+        <v>0.55</v>
       </c>
       <c r="K22" t="n">
-        <v>4.5</v>
+        <v>3.27</v>
       </c>
       <c r="L22" t="n">
-        <v>3</v>
+        <v>1.79</v>
       </c>
       <c r="M22" t="n">
-        <v>10.5</v>
+        <v>7.64</v>
       </c>
       <c r="N22" t="n">
-        <v>3.7</v>
+        <v>2.06</v>
       </c>
       <c r="O22" t="n">
-        <v>118.5</v>
+        <v>73.73</v>
       </c>
       <c r="P22" t="n">
-        <v>31.08</v>
+        <v>28.44</v>
       </c>
       <c r="Q22" t="n">
-        <v>1.25</v>
+        <v>0.55</v>
       </c>
       <c r="R22" t="n">
-        <v>1.26</v>
+        <v>0.93</v>
       </c>
       <c r="S22" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
@@ -1862,10 +1862,10 @@
         <v>40</v>
       </c>
       <c r="B23" t="n">
-        <v>1.75</v>
+        <v>3.25</v>
       </c>
       <c r="C23" t="n">
-        <v>0.46</v>
+        <v>1.71</v>
       </c>
       <c r="D23" t="n">
         <v>1</v>
@@ -1880,40 +1880,40 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="I23" t="n">
-        <v>1.75</v>
+        <v>1.5</v>
       </c>
       <c r="J23" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="K23" t="n">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L23" t="n">
-        <v>1.85</v>
+        <v>3</v>
       </c>
       <c r="M23" t="n">
-        <v>6.25</v>
+        <v>10.5</v>
       </c>
       <c r="N23" t="n">
-        <v>4.5</v>
+        <v>3.7</v>
       </c>
       <c r="O23" t="n">
-        <v>73.38</v>
+        <v>118.5</v>
       </c>
       <c r="P23" t="n">
-        <v>44.11</v>
+        <v>31.08</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.25</v>
+        <v>1.25</v>
       </c>
       <c r="R23" t="n">
-        <v>0.46</v>
+        <v>1.26</v>
       </c>
       <c r="S23" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
@@ -1921,58 +1921,58 @@
         <v>41</v>
       </c>
       <c r="B24" t="n">
-        <v>1.89</v>
+        <v>1.75</v>
       </c>
       <c r="C24" t="n">
-        <v>1.45</v>
+        <v>0.46</v>
       </c>
       <c r="D24" t="n">
-        <v>0.78</v>
+        <v>1</v>
       </c>
       <c r="E24" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="F24" t="n">
-        <v>0.44</v>
+        <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>0.22</v>
+        <v>0</v>
       </c>
       <c r="H24" t="n">
-        <v>0.44</v>
+        <v>0.75</v>
       </c>
       <c r="I24" t="n">
-        <v>0.53</v>
+        <v>1.75</v>
       </c>
       <c r="J24" t="n">
-        <v>0.44</v>
+        <v>0.25</v>
       </c>
       <c r="K24" t="n">
-        <v>2.56</v>
+        <v>2.5</v>
       </c>
       <c r="L24" t="n">
-        <v>1.33</v>
+        <v>1.85</v>
       </c>
       <c r="M24" t="n">
-        <v>8.22</v>
+        <v>6.25</v>
       </c>
       <c r="N24" t="n">
-        <v>5.7</v>
+        <v>4.5</v>
       </c>
       <c r="O24" t="n">
-        <v>92.22</v>
+        <v>73.38</v>
       </c>
       <c r="P24" t="n">
-        <v>35.45</v>
+        <v>44.11</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.67</v>
+        <v>0.25</v>
       </c>
       <c r="R24" t="n">
-        <v>1</v>
+        <v>0.46</v>
       </c>
       <c r="S24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25">
@@ -1980,58 +1980,58 @@
         <v>42</v>
       </c>
       <c r="B25" t="n">
-        <v>0.46</v>
+        <v>1.89</v>
       </c>
       <c r="C25" t="n">
-        <v>0.81</v>
+        <v>1.45</v>
       </c>
       <c r="D25" t="n">
-        <v>0.31</v>
+        <v>0.78</v>
       </c>
       <c r="E25" t="n">
-        <v>1.53</v>
+        <v>0.22</v>
       </c>
       <c r="F25" t="n">
-        <v>1.48</v>
+        <v>0.44</v>
       </c>
       <c r="G25" t="n">
-        <v>0.7</v>
+        <v>0.22</v>
       </c>
       <c r="H25" t="n">
-        <v>0.51</v>
+        <v>0.44</v>
       </c>
       <c r="I25" t="n">
-        <v>0.88</v>
+        <v>0.53</v>
       </c>
       <c r="J25" t="n">
-        <v>0.34</v>
+        <v>0.44</v>
       </c>
       <c r="K25" t="n">
-        <v>2.5</v>
+        <v>2.56</v>
       </c>
       <c r="L25" t="n">
-        <v>2.11</v>
+        <v>1.33</v>
       </c>
       <c r="M25" t="n">
-        <v>6.39</v>
+        <v>8.22</v>
       </c>
       <c r="N25" t="n">
-        <v>2.68</v>
+        <v>5.7</v>
       </c>
       <c r="O25" t="n">
-        <v>78.2</v>
+        <v>92.22</v>
       </c>
       <c r="P25" t="n">
-        <v>34.44</v>
+        <v>35.45</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.4</v>
+        <v>0.67</v>
       </c>
       <c r="R25" t="n">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="S25" t="n">
-        <v>200</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26">
@@ -2039,58 +2039,58 @@
         <v>43</v>
       </c>
       <c r="B26" t="n">
-        <v>0.62</v>
+        <v>0.46</v>
       </c>
       <c r="C26" t="n">
-        <v>0.74</v>
+        <v>0.81</v>
       </c>
       <c r="D26" t="n">
-        <v>0.5</v>
+        <v>0.31</v>
       </c>
       <c r="E26" t="n">
-        <v>0.25</v>
+        <v>1.53</v>
       </c>
       <c r="F26" t="n">
-        <v>0.46</v>
+        <v>1.48</v>
       </c>
       <c r="G26" t="n">
-        <v>0.25</v>
+        <v>0.7</v>
       </c>
       <c r="H26" t="n">
-        <v>1.5</v>
+        <v>0.51</v>
       </c>
       <c r="I26" t="n">
-        <v>1.93</v>
+        <v>0.88</v>
       </c>
       <c r="J26" t="n">
-        <v>0.62</v>
+        <v>0.34</v>
       </c>
       <c r="K26" t="n">
-        <v>2.38</v>
+        <v>2.5</v>
       </c>
       <c r="L26" t="n">
-        <v>2.45</v>
+        <v>2.11</v>
       </c>
       <c r="M26" t="n">
-        <v>7.5</v>
+        <v>6.39</v>
       </c>
       <c r="N26" t="n">
-        <v>4.84</v>
+        <v>2.68</v>
       </c>
       <c r="O26" t="n">
-        <v>85.38</v>
+        <v>78.2</v>
       </c>
       <c r="P26" t="n">
-        <v>38.78</v>
+        <v>34.44</v>
       </c>
       <c r="Q26" t="n">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="R26" t="n">
-        <v>2.07</v>
+        <v>0.7</v>
       </c>
       <c r="S26" t="n">
-        <v>8</v>
+        <v>200</v>
       </c>
     </row>
     <row r="27">
@@ -2098,58 +2098,58 @@
         <v>44</v>
       </c>
       <c r="B27" t="n">
-        <v>0.77</v>
+        <v>0.62</v>
       </c>
       <c r="C27" t="n">
-        <v>0.93</v>
+        <v>0.74</v>
       </c>
       <c r="D27" t="n">
-        <v>0.54</v>
+        <v>0.5</v>
       </c>
       <c r="E27" t="n">
-        <v>0.69</v>
+        <v>0.25</v>
       </c>
       <c r="F27" t="n">
-        <v>1.18</v>
+        <v>0.46</v>
       </c>
       <c r="G27" t="n">
-        <v>0.38</v>
+        <v>0.25</v>
       </c>
       <c r="H27" t="n">
-        <v>1.69</v>
+        <v>1.5</v>
       </c>
       <c r="I27" t="n">
-        <v>2.25</v>
+        <v>1.93</v>
       </c>
       <c r="J27" t="n">
-        <v>0.54</v>
+        <v>0.62</v>
       </c>
       <c r="K27" t="n">
-        <v>3.15</v>
+        <v>2.38</v>
       </c>
       <c r="L27" t="n">
-        <v>3.11</v>
+        <v>2.45</v>
       </c>
       <c r="M27" t="n">
-        <v>9.46</v>
+        <v>7.5</v>
       </c>
       <c r="N27" t="n">
-        <v>4.03</v>
+        <v>4.84</v>
       </c>
       <c r="O27" t="n">
-        <v>103.92</v>
+        <v>85.38</v>
       </c>
       <c r="P27" t="n">
-        <v>39.52</v>
+        <v>38.78</v>
       </c>
       <c r="Q27" t="n">
-        <v>1.23</v>
+        <v>1</v>
       </c>
       <c r="R27" t="n">
-        <v>1.09</v>
+        <v>2.07</v>
       </c>
       <c r="S27" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -2157,58 +2157,58 @@
         <v>45</v>
       </c>
       <c r="B28" t="n">
-        <v>2.18</v>
+        <v>0.77</v>
       </c>
       <c r="C28" t="n">
-        <v>2.23</v>
+        <v>0.93</v>
       </c>
       <c r="D28" t="n">
-        <v>0.73</v>
+        <v>0.54</v>
       </c>
       <c r="E28" t="n">
-        <v>0.09</v>
+        <v>0.69</v>
       </c>
       <c r="F28" t="n">
-        <v>0.3</v>
+        <v>1.18</v>
       </c>
       <c r="G28" t="n">
-        <v>0.09</v>
+        <v>0.38</v>
       </c>
       <c r="H28" t="n">
-        <v>1.18</v>
+        <v>1.69</v>
       </c>
       <c r="I28" t="n">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="J28" t="n">
-        <v>0.55</v>
+        <v>0.54</v>
       </c>
       <c r="K28" t="n">
-        <v>3.45</v>
+        <v>3.15</v>
       </c>
       <c r="L28" t="n">
-        <v>2.16</v>
+        <v>3.11</v>
       </c>
       <c r="M28" t="n">
-        <v>7.45</v>
+        <v>9.46</v>
       </c>
       <c r="N28" t="n">
-        <v>2.62</v>
+        <v>4.03</v>
       </c>
       <c r="O28" t="n">
-        <v>92.09</v>
+        <v>103.92</v>
       </c>
       <c r="P28" t="n">
-        <v>41.49</v>
+        <v>39.52</v>
       </c>
       <c r="Q28" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="R28" t="n">
         <v>1.09</v>
       </c>
-      <c r="R28" t="n">
-        <v>1.81</v>
-      </c>
       <c r="S28" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29">
@@ -2216,58 +2216,58 @@
         <v>46</v>
       </c>
       <c r="B29" t="n">
-        <v>0.67</v>
+        <v>2.18</v>
       </c>
       <c r="C29" t="n">
-        <v>0.58</v>
+        <v>2.23</v>
       </c>
       <c r="D29" t="n">
-        <v>0.67</v>
+        <v>0.73</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="G29" t="n">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="H29" t="n">
-        <v>0.33</v>
+        <v>1.18</v>
       </c>
       <c r="I29" t="n">
-        <v>0.58</v>
+        <v>1.4</v>
       </c>
       <c r="J29" t="n">
-        <v>0.33</v>
+        <v>0.55</v>
       </c>
       <c r="K29" t="n">
-        <v>1</v>
+        <v>3.45</v>
       </c>
       <c r="L29" t="n">
-        <v>1</v>
+        <v>2.16</v>
       </c>
       <c r="M29" t="n">
-        <v>6.33</v>
+        <v>7.45</v>
       </c>
       <c r="N29" t="n">
-        <v>3.51</v>
+        <v>2.62</v>
       </c>
       <c r="O29" t="n">
-        <v>82.67</v>
+        <v>92.09</v>
       </c>
       <c r="P29" t="n">
-        <v>59.35</v>
+        <v>41.49</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.33</v>
+        <v>1.09</v>
       </c>
       <c r="R29" t="n">
-        <v>0.58</v>
+        <v>1.81</v>
       </c>
       <c r="S29" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30">
@@ -2275,22 +2275,22 @@
         <v>47</v>
       </c>
       <c r="B30" t="n">
-        <v>2.33</v>
+        <v>0.67</v>
       </c>
       <c r="C30" t="n">
-        <v>1.15</v>
+        <v>0.58</v>
       </c>
       <c r="D30" t="n">
-        <v>1</v>
+        <v>0.67</v>
       </c>
       <c r="E30" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>0.58</v>
+        <v>0</v>
       </c>
       <c r="G30" t="n">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="H30" t="n">
         <v>0.33</v>
@@ -2302,28 +2302,28 @@
         <v>0.33</v>
       </c>
       <c r="K30" t="n">
-        <v>3.33</v>
+        <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>1.53</v>
+        <v>1</v>
       </c>
       <c r="M30" t="n">
-        <v>10</v>
+        <v>6.33</v>
       </c>
       <c r="N30" t="n">
-        <v>4.58</v>
+        <v>3.51</v>
       </c>
       <c r="O30" t="n">
-        <v>113.33</v>
+        <v>82.67</v>
       </c>
       <c r="P30" t="n">
-        <v>55.9</v>
+        <v>59.35</v>
       </c>
       <c r="Q30" t="n">
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="R30" t="n">
-        <v>1</v>
+        <v>0.58</v>
       </c>
       <c r="S30" t="n">
         <v>3</v>
@@ -2334,58 +2334,58 @@
         <v>48</v>
       </c>
       <c r="B31" t="n">
-        <v>1.2</v>
+        <v>2.33</v>
       </c>
       <c r="C31" t="n">
-        <v>1.32</v>
+        <v>1.15</v>
       </c>
       <c r="D31" t="n">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.13</v>
+        <v>0.67</v>
       </c>
       <c r="F31" t="n">
-        <v>0.35</v>
+        <v>0.58</v>
       </c>
       <c r="G31" t="n">
-        <v>0.13</v>
+        <v>0.67</v>
       </c>
       <c r="H31" t="n">
-        <v>0.6</v>
+        <v>0.33</v>
       </c>
       <c r="I31" t="n">
-        <v>1.06</v>
+        <v>0.58</v>
       </c>
       <c r="J31" t="n">
         <v>0.33</v>
       </c>
       <c r="K31" t="n">
-        <v>1.93</v>
+        <v>3.33</v>
       </c>
       <c r="L31" t="n">
-        <v>1.39</v>
+        <v>1.53</v>
       </c>
       <c r="M31" t="n">
-        <v>6.93</v>
+        <v>10</v>
       </c>
       <c r="N31" t="n">
-        <v>3.59</v>
+        <v>4.58</v>
       </c>
       <c r="O31" t="n">
-        <v>86.6</v>
+        <v>113.33</v>
       </c>
       <c r="P31" t="n">
-        <v>40.45</v>
+        <v>55.9</v>
       </c>
       <c r="Q31" t="n">
         <v>1</v>
       </c>
       <c r="R31" t="n">
-        <v>1.51</v>
+        <v>1</v>
       </c>
       <c r="S31" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -2393,58 +2393,58 @@
         <v>49</v>
       </c>
       <c r="B32" t="n">
-        <v>2.75</v>
+        <v>1.2</v>
       </c>
       <c r="C32" t="n">
-        <v>1.49</v>
+        <v>1.32</v>
       </c>
       <c r="D32" t="n">
-        <v>0.88</v>
+        <v>0.6</v>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="F32" t="n">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="G32" t="n">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="H32" t="n">
-        <v>1.12</v>
+        <v>0.6</v>
       </c>
       <c r="I32" t="n">
-        <v>1.64</v>
+        <v>1.06</v>
       </c>
       <c r="J32" t="n">
-        <v>0.38</v>
+        <v>0.33</v>
       </c>
       <c r="K32" t="n">
-        <v>3.88</v>
+        <v>1.93</v>
       </c>
       <c r="L32" t="n">
-        <v>1.96</v>
+        <v>1.39</v>
       </c>
       <c r="M32" t="n">
-        <v>7.75</v>
+        <v>6.93</v>
       </c>
       <c r="N32" t="n">
-        <v>4.06</v>
+        <v>3.59</v>
       </c>
       <c r="O32" t="n">
-        <v>105.62</v>
+        <v>86.6</v>
       </c>
       <c r="P32" t="n">
-        <v>56.67</v>
+        <v>40.45</v>
       </c>
       <c r="Q32" t="n">
-        <v>1.88</v>
+        <v>1</v>
       </c>
       <c r="R32" t="n">
-        <v>3.04</v>
+        <v>1.51</v>
       </c>
       <c r="S32" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33">
@@ -2452,58 +2452,58 @@
         <v>50</v>
       </c>
       <c r="B33" t="n">
-        <v>2.2</v>
+        <v>2.75</v>
       </c>
       <c r="C33" t="n">
-        <v>1.23</v>
+        <v>1.49</v>
       </c>
       <c r="D33" t="n">
-        <v>0.9</v>
+        <v>0.88</v>
       </c>
       <c r="E33" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F33" t="n">
-        <v>0.32</v>
+        <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1</v>
+        <v>1.12</v>
       </c>
       <c r="I33" t="n">
-        <v>0.32</v>
+        <v>1.64</v>
       </c>
       <c r="J33" t="n">
-        <v>0.1</v>
+        <v>0.38</v>
       </c>
       <c r="K33" t="n">
-        <v>2.4</v>
+        <v>3.88</v>
       </c>
       <c r="L33" t="n">
-        <v>1.26</v>
+        <v>1.96</v>
       </c>
       <c r="M33" t="n">
-        <v>9.7</v>
+        <v>7.75</v>
       </c>
       <c r="N33" t="n">
-        <v>6.22</v>
+        <v>4.06</v>
       </c>
       <c r="O33" t="n">
-        <v>99.5</v>
+        <v>105.62</v>
       </c>
       <c r="P33" t="n">
-        <v>45.63</v>
+        <v>56.67</v>
       </c>
       <c r="Q33" t="n">
-        <v>0.7</v>
+        <v>1.88</v>
       </c>
       <c r="R33" t="n">
-        <v>1.34</v>
+        <v>3.04</v>
       </c>
       <c r="S33" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
@@ -2511,58 +2511,58 @@
         <v>51</v>
       </c>
       <c r="B34" t="n">
-        <v>0.6</v>
+        <v>2.2</v>
       </c>
       <c r="C34" t="n">
-        <v>0.83</v>
+        <v>1.23</v>
       </c>
       <c r="D34" t="n">
-        <v>0.47</v>
+        <v>0.9</v>
       </c>
       <c r="E34" t="n">
-        <v>1.33</v>
+        <v>0.1</v>
       </c>
       <c r="F34" t="n">
-        <v>1.95</v>
+        <v>0.32</v>
       </c>
       <c r="G34" t="n">
-        <v>0.47</v>
+        <v>0.1</v>
       </c>
       <c r="H34" t="n">
-        <v>1.47</v>
+        <v>0.1</v>
       </c>
       <c r="I34" t="n">
-        <v>1.51</v>
+        <v>0.32</v>
       </c>
       <c r="J34" t="n">
-        <v>0.67</v>
+        <v>0.1</v>
       </c>
       <c r="K34" t="n">
-        <v>3.4</v>
+        <v>2.4</v>
       </c>
       <c r="L34" t="n">
-        <v>2.41</v>
+        <v>1.26</v>
       </c>
       <c r="M34" t="n">
-        <v>7.07</v>
+        <v>9.7</v>
       </c>
       <c r="N34" t="n">
-        <v>3.99</v>
+        <v>6.22</v>
       </c>
       <c r="O34" t="n">
-        <v>87.93</v>
+        <v>99.5</v>
       </c>
       <c r="P34" t="n">
-        <v>43.97</v>
+        <v>45.63</v>
       </c>
       <c r="Q34" t="n">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="R34" t="n">
-        <v>1.41</v>
+        <v>1.34</v>
       </c>
       <c r="S34" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -2570,58 +2570,58 @@
         <v>52</v>
       </c>
       <c r="B35" t="n">
-        <v>2.45</v>
+        <v>0.6</v>
       </c>
       <c r="C35" t="n">
-        <v>1.21</v>
+        <v>0.83</v>
       </c>
       <c r="D35" t="n">
-        <v>0.91</v>
+        <v>0.47</v>
       </c>
       <c r="E35" t="n">
-        <v>0.55</v>
+        <v>1.33</v>
       </c>
       <c r="F35" t="n">
-        <v>0.82</v>
+        <v>1.95</v>
       </c>
       <c r="G35" t="n">
-        <v>0.36</v>
+        <v>0.47</v>
       </c>
       <c r="H35" t="n">
-        <v>0.55</v>
+        <v>1.47</v>
       </c>
       <c r="I35" t="n">
-        <v>0.82</v>
+        <v>1.51</v>
       </c>
       <c r="J35" t="n">
-        <v>0.36</v>
+        <v>0.67</v>
       </c>
       <c r="K35" t="n">
-        <v>3.55</v>
+        <v>3.4</v>
       </c>
       <c r="L35" t="n">
-        <v>1.86</v>
+        <v>2.41</v>
       </c>
       <c r="M35" t="n">
-        <v>5.91</v>
+        <v>7.07</v>
       </c>
       <c r="N35" t="n">
-        <v>4.3</v>
+        <v>3.99</v>
       </c>
       <c r="O35" t="n">
-        <v>77.18</v>
+        <v>87.93</v>
       </c>
       <c r="P35" t="n">
-        <v>41.66</v>
+        <v>43.97</v>
       </c>
       <c r="Q35" t="n">
-        <v>0.27</v>
+        <v>1</v>
       </c>
       <c r="R35" t="n">
-        <v>0.65</v>
+        <v>1.41</v>
       </c>
       <c r="S35" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36">
@@ -2629,58 +2629,58 @@
         <v>53</v>
       </c>
       <c r="B36" t="n">
-        <v>1.57</v>
+        <v>2.45</v>
       </c>
       <c r="C36" t="n">
-        <v>0.79</v>
+        <v>1.21</v>
       </c>
       <c r="D36" t="n">
-        <v>0.86</v>
+        <v>0.91</v>
       </c>
       <c r="E36" t="n">
-        <v>0.14</v>
+        <v>0.55</v>
       </c>
       <c r="F36" t="n">
-        <v>0.38</v>
+        <v>0.82</v>
       </c>
       <c r="G36" t="n">
-        <v>0.14</v>
+        <v>0.36</v>
       </c>
       <c r="H36" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0.82</v>
+      </c>
+      <c r="J36" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K36" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="L36" t="n">
         <v>1.86</v>
       </c>
-      <c r="I36" t="n">
-        <v>2.34</v>
-      </c>
-      <c r="J36" t="n">
-        <v>0.57</v>
-      </c>
-      <c r="K36" t="n">
-        <v>3.57</v>
-      </c>
-      <c r="L36" t="n">
-        <v>1.9</v>
-      </c>
       <c r="M36" t="n">
-        <v>10.57</v>
+        <v>5.91</v>
       </c>
       <c r="N36" t="n">
-        <v>7.41</v>
+        <v>4.3</v>
       </c>
       <c r="O36" t="n">
-        <v>119.29</v>
+        <v>77.18</v>
       </c>
       <c r="P36" t="n">
-        <v>72.73</v>
+        <v>41.66</v>
       </c>
       <c r="Q36" t="n">
-        <v>1.71</v>
+        <v>0.27</v>
       </c>
       <c r="R36" t="n">
-        <v>1.5</v>
+        <v>0.65</v>
       </c>
       <c r="S36" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37">
@@ -2688,58 +2688,58 @@
         <v>54</v>
       </c>
       <c r="B37" t="n">
-        <v>1.89</v>
+        <v>1.57</v>
       </c>
       <c r="C37" t="n">
-        <v>0.78</v>
+        <v>0.79</v>
       </c>
       <c r="D37" t="n">
-        <v>1</v>
+        <v>0.86</v>
       </c>
       <c r="E37" t="n">
-        <v>0.33</v>
+        <v>0.14</v>
       </c>
       <c r="F37" t="n">
-        <v>0.71</v>
+        <v>0.38</v>
       </c>
       <c r="G37" t="n">
-        <v>0.22</v>
+        <v>0.14</v>
       </c>
       <c r="H37" t="n">
-        <v>1.11</v>
+        <v>1.86</v>
       </c>
       <c r="I37" t="n">
-        <v>1.05</v>
+        <v>2.34</v>
       </c>
       <c r="J37" t="n">
-        <v>0.67</v>
+        <v>0.57</v>
       </c>
       <c r="K37" t="n">
-        <v>3.33</v>
+        <v>3.57</v>
       </c>
       <c r="L37" t="n">
-        <v>1.12</v>
+        <v>1.9</v>
       </c>
       <c r="M37" t="n">
-        <v>8.11</v>
+        <v>10.57</v>
       </c>
       <c r="N37" t="n">
-        <v>3.82</v>
+        <v>7.41</v>
       </c>
       <c r="O37" t="n">
-        <v>87.78</v>
+        <v>119.29</v>
       </c>
       <c r="P37" t="n">
-        <v>36.52</v>
+        <v>72.73</v>
       </c>
       <c r="Q37" t="n">
-        <v>1.11</v>
+        <v>1.71</v>
       </c>
       <c r="R37" t="n">
-        <v>1.05</v>
+        <v>1.5</v>
       </c>
       <c r="S37" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
@@ -2747,58 +2747,58 @@
         <v>55</v>
       </c>
       <c r="B38" t="n">
-        <v>0.25</v>
+        <v>1.89</v>
       </c>
       <c r="C38" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="F38" t="n">
         <v>0.71</v>
       </c>
-      <c r="D38" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="E38" t="n">
+      <c r="G38" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="I38" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="J38" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="K38" t="n">
+        <v>3.33</v>
+      </c>
+      <c r="L38" t="n">
         <v>1.12</v>
       </c>
-      <c r="F38" t="n">
-        <v>0.99</v>
-      </c>
-      <c r="G38" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="I38" t="n">
-        <v>0.74</v>
-      </c>
-      <c r="J38" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K38" t="n">
-        <v>2</v>
-      </c>
-      <c r="L38" t="n">
-        <v>1.6</v>
-      </c>
       <c r="M38" t="n">
-        <v>7.75</v>
+        <v>8.11</v>
       </c>
       <c r="N38" t="n">
-        <v>5.99</v>
+        <v>3.82</v>
       </c>
       <c r="O38" t="n">
-        <v>93</v>
+        <v>87.78</v>
       </c>
       <c r="P38" t="n">
-        <v>43.59</v>
+        <v>36.52</v>
       </c>
       <c r="Q38" t="n">
-        <v>0.38</v>
+        <v>1.11</v>
       </c>
       <c r="R38" t="n">
-        <v>0.52</v>
+        <v>1.05</v>
       </c>
       <c r="S38" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39">
@@ -2806,58 +2806,58 @@
         <v>56</v>
       </c>
       <c r="B39" t="n">
-        <v>1.36</v>
+        <v>0.25</v>
       </c>
       <c r="C39" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E39" t="n">
         <v>1.12</v>
       </c>
-      <c r="D39" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="E39" t="n">
-        <v>1.73</v>
-      </c>
       <c r="F39" t="n">
-        <v>1.56</v>
+        <v>0.99</v>
       </c>
       <c r="G39" t="n">
-        <v>0.73</v>
+        <v>0.75</v>
       </c>
       <c r="H39" t="n">
-        <v>1.55</v>
+        <v>0.62</v>
       </c>
       <c r="I39" t="n">
-        <v>0.69</v>
+        <v>0.74</v>
       </c>
       <c r="J39" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="K39" t="n">
-        <v>4.64</v>
+        <v>2</v>
       </c>
       <c r="L39" t="n">
-        <v>1.75</v>
+        <v>1.6</v>
       </c>
       <c r="M39" t="n">
-        <v>6</v>
+        <v>7.75</v>
       </c>
       <c r="N39" t="n">
-        <v>2.61</v>
+        <v>5.99</v>
       </c>
       <c r="O39" t="n">
-        <v>65.82</v>
+        <v>93</v>
       </c>
       <c r="P39" t="n">
-        <v>26.26</v>
+        <v>43.59</v>
       </c>
       <c r="Q39" t="n">
-        <v>0.45</v>
+        <v>0.38</v>
       </c>
       <c r="R39" t="n">
-        <v>0.69</v>
+        <v>0.52</v>
       </c>
       <c r="S39" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
@@ -2865,58 +2865,58 @@
         <v>57</v>
       </c>
       <c r="B40" t="n">
-        <v>2.38</v>
+        <v>1.36</v>
       </c>
       <c r="C40" t="n">
-        <v>1.77</v>
+        <v>1.12</v>
       </c>
       <c r="D40" t="n">
-        <v>0.88</v>
+        <v>0.73</v>
       </c>
       <c r="E40" t="n">
-        <v>0.38</v>
+        <v>1.73</v>
       </c>
       <c r="F40" t="n">
-        <v>0.74</v>
+        <v>1.56</v>
       </c>
       <c r="G40" t="n">
-        <v>0.25</v>
+        <v>0.73</v>
       </c>
       <c r="H40" t="n">
-        <v>1.25</v>
+        <v>1.55</v>
       </c>
       <c r="I40" t="n">
-        <v>1.16</v>
+        <v>0.69</v>
       </c>
       <c r="J40" t="n">
-        <v>0.62</v>
+        <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>4</v>
+        <v>4.64</v>
       </c>
       <c r="L40" t="n">
-        <v>1.69</v>
+        <v>1.75</v>
       </c>
       <c r="M40" t="n">
-        <v>5.12</v>
+        <v>6</v>
       </c>
       <c r="N40" t="n">
-        <v>2.53</v>
+        <v>2.61</v>
       </c>
       <c r="O40" t="n">
-        <v>70.12</v>
+        <v>65.82</v>
       </c>
       <c r="P40" t="n">
-        <v>31.53</v>
+        <v>26.26</v>
       </c>
       <c r="Q40" t="n">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="R40" t="n">
-        <v>0.76</v>
+        <v>0.69</v>
       </c>
       <c r="S40" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41">
@@ -2924,58 +2924,58 @@
         <v>58</v>
       </c>
       <c r="B41" t="n">
-        <v>0.8</v>
+        <v>2.38</v>
       </c>
       <c r="C41" t="n">
-        <v>0.86</v>
+        <v>1.77</v>
       </c>
       <c r="D41" t="n">
-        <v>0.53</v>
+        <v>0.88</v>
       </c>
       <c r="E41" t="n">
-        <v>0.87</v>
+        <v>0.38</v>
       </c>
       <c r="F41" t="n">
-        <v>1.36</v>
+        <v>0.74</v>
       </c>
       <c r="G41" t="n">
-        <v>0.47</v>
+        <v>0.25</v>
       </c>
       <c r="H41" t="n">
-        <v>0.8</v>
+        <v>1.25</v>
       </c>
       <c r="I41" t="n">
-        <v>0.77</v>
+        <v>1.16</v>
       </c>
       <c r="J41" t="n">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="K41" t="n">
-        <v>2.47</v>
+        <v>4</v>
       </c>
       <c r="L41" t="n">
-        <v>1.36</v>
+        <v>1.69</v>
       </c>
       <c r="M41" t="n">
-        <v>5.6</v>
+        <v>5.12</v>
       </c>
       <c r="N41" t="n">
-        <v>3.25</v>
+        <v>2.53</v>
       </c>
       <c r="O41" t="n">
-        <v>69.13</v>
+        <v>70.12</v>
       </c>
       <c r="P41" t="n">
-        <v>35.65</v>
+        <v>31.53</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.07</v>
+        <v>0.5</v>
       </c>
       <c r="R41" t="n">
-        <v>0.26</v>
+        <v>0.76</v>
       </c>
       <c r="S41" t="n">
-        <v>15</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
@@ -2983,58 +2983,58 @@
         <v>59</v>
       </c>
       <c r="B42" t="n">
-        <v>0.89</v>
+        <v>0.8</v>
       </c>
       <c r="C42" t="n">
-        <v>0.93</v>
+        <v>0.86</v>
       </c>
       <c r="D42" t="n">
-        <v>0.67</v>
+        <v>0.53</v>
       </c>
       <c r="E42" t="n">
-        <v>1.56</v>
+        <v>0.87</v>
       </c>
       <c r="F42" t="n">
-        <v>1.42</v>
+        <v>1.36</v>
       </c>
       <c r="G42" t="n">
-        <v>0.67</v>
+        <v>0.47</v>
       </c>
       <c r="H42" t="n">
-        <v>1.44</v>
+        <v>0.8</v>
       </c>
       <c r="I42" t="n">
-        <v>1.51</v>
+        <v>0.77</v>
       </c>
       <c r="J42" t="n">
-        <v>0.67</v>
+        <v>0.6</v>
       </c>
       <c r="K42" t="n">
-        <v>3.89</v>
+        <v>2.47</v>
       </c>
       <c r="L42" t="n">
-        <v>2.47</v>
+        <v>1.36</v>
       </c>
       <c r="M42" t="n">
-        <v>7.11</v>
+        <v>5.6</v>
       </c>
       <c r="N42" t="n">
-        <v>3.37</v>
+        <v>3.25</v>
       </c>
       <c r="O42" t="n">
-        <v>73.33</v>
+        <v>69.13</v>
       </c>
       <c r="P42" t="n">
-        <v>30.45</v>
+        <v>35.65</v>
       </c>
       <c r="Q42" t="n">
-        <v>0.67</v>
+        <v>0.07</v>
       </c>
       <c r="R42" t="n">
-        <v>1.32</v>
+        <v>0.26</v>
       </c>
       <c r="S42" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43">
@@ -3042,58 +3042,58 @@
         <v>60</v>
       </c>
       <c r="B43" t="n">
-        <v>0.77</v>
+        <v>0.89</v>
       </c>
       <c r="C43" t="n">
-        <v>1.01</v>
+        <v>0.93</v>
       </c>
       <c r="D43" t="n">
-        <v>0.48</v>
+        <v>0.67</v>
       </c>
       <c r="E43" t="n">
-        <v>1.82</v>
+        <v>1.56</v>
       </c>
       <c r="F43" t="n">
-        <v>1.27</v>
+        <v>1.42</v>
       </c>
       <c r="G43" t="n">
-        <v>0.9</v>
+        <v>0.67</v>
       </c>
       <c r="H43" t="n">
-        <v>2.11</v>
+        <v>1.44</v>
       </c>
       <c r="I43" t="n">
-        <v>1.46</v>
+        <v>1.51</v>
       </c>
       <c r="J43" t="n">
-        <v>0.88</v>
+        <v>0.67</v>
       </c>
       <c r="K43" t="n">
-        <v>4.7</v>
+        <v>3.89</v>
       </c>
       <c r="L43" t="n">
-        <v>2.31</v>
+        <v>2.47</v>
       </c>
       <c r="M43" t="n">
-        <v>6.35</v>
+        <v>7.11</v>
       </c>
       <c r="N43" t="n">
-        <v>2.68</v>
+        <v>3.37</v>
       </c>
       <c r="O43" t="n">
-        <v>83.67</v>
+        <v>73.33</v>
       </c>
       <c r="P43" t="n">
-        <v>32.94</v>
+        <v>30.45</v>
       </c>
       <c r="Q43" t="n">
-        <v>0.38</v>
+        <v>0.67</v>
       </c>
       <c r="R43" t="n">
-        <v>0.67</v>
+        <v>1.32</v>
       </c>
       <c r="S43" t="n">
-        <v>198</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44">
@@ -3101,58 +3101,58 @@
         <v>61</v>
       </c>
       <c r="B44" t="n">
-        <v>0.35</v>
+        <v>0.77</v>
       </c>
       <c r="C44" t="n">
-        <v>0.79</v>
+        <v>1.01</v>
       </c>
       <c r="D44" t="n">
-        <v>0.21</v>
+        <v>0.48</v>
       </c>
       <c r="E44" t="n">
-        <v>1.2</v>
+        <v>1.82</v>
       </c>
       <c r="F44" t="n">
-        <v>1.13</v>
+        <v>1.27</v>
       </c>
       <c r="G44" t="n">
-        <v>0.66</v>
+        <v>0.9</v>
       </c>
       <c r="H44" t="n">
-        <v>0.86</v>
+        <v>2.11</v>
       </c>
       <c r="I44" t="n">
-        <v>1.11</v>
+        <v>1.46</v>
       </c>
       <c r="J44" t="n">
-        <v>0.52</v>
+        <v>0.88</v>
       </c>
       <c r="K44" t="n">
-        <v>2.41</v>
+        <v>4.7</v>
       </c>
       <c r="L44" t="n">
-        <v>1.62</v>
+        <v>2.31</v>
       </c>
       <c r="M44" t="n">
-        <v>5.1</v>
+        <v>6.35</v>
       </c>
       <c r="N44" t="n">
-        <v>2.44</v>
+        <v>2.68</v>
       </c>
       <c r="O44" t="n">
-        <v>58.99</v>
+        <v>83.67</v>
       </c>
       <c r="P44" t="n">
-        <v>25.32</v>
+        <v>32.94</v>
       </c>
       <c r="Q44" t="n">
-        <v>0.47</v>
+        <v>0.38</v>
       </c>
       <c r="R44" t="n">
-        <v>0.71</v>
+        <v>0.67</v>
       </c>
       <c r="S44" t="n">
-        <v>354</v>
+        <v>198</v>
       </c>
     </row>
     <row r="45">
@@ -3160,58 +3160,58 @@
         <v>62</v>
       </c>
       <c r="B45" t="n">
-        <v>2.39</v>
+        <v>0.35</v>
       </c>
       <c r="C45" t="n">
-        <v>1.67</v>
+        <v>0.79</v>
       </c>
       <c r="D45" t="n">
-        <v>0.88</v>
+        <v>0.21</v>
       </c>
       <c r="E45" t="n">
-        <v>0.14</v>
+        <v>1.2</v>
       </c>
       <c r="F45" t="n">
-        <v>0.41</v>
+        <v>1.13</v>
       </c>
       <c r="G45" t="n">
-        <v>0.12</v>
+        <v>0.66</v>
       </c>
       <c r="H45" t="n">
-        <v>1.08</v>
+        <v>0.86</v>
       </c>
       <c r="I45" t="n">
-        <v>1.25</v>
+        <v>1.11</v>
       </c>
       <c r="J45" t="n">
-        <v>0.58</v>
+        <v>0.52</v>
       </c>
       <c r="K45" t="n">
-        <v>3.61</v>
+        <v>2.41</v>
       </c>
       <c r="L45" t="n">
-        <v>2.07</v>
+        <v>1.62</v>
       </c>
       <c r="M45" t="n">
-        <v>6.96</v>
+        <v>5.1</v>
       </c>
       <c r="N45" t="n">
-        <v>3.25</v>
+        <v>2.44</v>
       </c>
       <c r="O45" t="n">
-        <v>92.56</v>
+        <v>58.99</v>
       </c>
       <c r="P45" t="n">
-        <v>37.21</v>
+        <v>25.32</v>
       </c>
       <c r="Q45" t="n">
-        <v>0.58</v>
+        <v>0.47</v>
       </c>
       <c r="R45" t="n">
-        <v>0.96</v>
+        <v>0.71</v>
       </c>
       <c r="S45" t="n">
-        <v>2311</v>
+        <v>354</v>
       </c>
     </row>
     <row r="46">
@@ -3219,58 +3219,58 @@
         <v>63</v>
       </c>
       <c r="B46" t="n">
-        <v>0.47</v>
+        <v>2.39</v>
       </c>
       <c r="C46" t="n">
-        <v>0.89</v>
+        <v>1.67</v>
       </c>
       <c r="D46" t="n">
-        <v>0.3</v>
+        <v>0.88</v>
       </c>
       <c r="E46" t="n">
-        <v>0.2</v>
+        <v>0.14</v>
       </c>
       <c r="F46" t="n">
-        <v>0.53</v>
+        <v>0.41</v>
       </c>
       <c r="G46" t="n">
-        <v>0.15</v>
+        <v>0.12</v>
       </c>
       <c r="H46" t="n">
-        <v>1.56</v>
+        <v>1.08</v>
       </c>
       <c r="I46" t="n">
-        <v>1.39</v>
+        <v>1.25</v>
       </c>
       <c r="J46" t="n">
-        <v>0.75</v>
+        <v>0.58</v>
       </c>
       <c r="K46" t="n">
-        <v>2.23</v>
+        <v>3.61</v>
       </c>
       <c r="L46" t="n">
-        <v>1.72</v>
+        <v>2.07</v>
       </c>
       <c r="M46" t="n">
-        <v>6.57</v>
+        <v>6.96</v>
       </c>
       <c r="N46" t="n">
-        <v>3.16</v>
+        <v>3.25</v>
       </c>
       <c r="O46" t="n">
-        <v>93.7</v>
+        <v>92.56</v>
       </c>
       <c r="P46" t="n">
-        <v>35.73</v>
+        <v>37.21</v>
       </c>
       <c r="Q46" t="n">
-        <v>0.78</v>
+        <v>0.57</v>
       </c>
       <c r="R46" t="n">
-        <v>1.12</v>
+        <v>0.96</v>
       </c>
       <c r="S46" t="n">
-        <v>2612</v>
+        <v>2311</v>
       </c>
     </row>
     <row r="47">
@@ -3278,58 +3278,58 @@
         <v>64</v>
       </c>
       <c r="B47" t="n">
-        <v>0.13</v>
+        <v>0.47</v>
       </c>
       <c r="C47" t="n">
-        <v>0.36</v>
+        <v>0.89</v>
       </c>
       <c r="D47" t="n">
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="E47" t="n">
-        <v>2.42</v>
+        <v>0.2</v>
       </c>
       <c r="F47" t="n">
-        <v>1.63</v>
+        <v>0.53</v>
       </c>
       <c r="G47" t="n">
-        <v>0.87</v>
+        <v>0.15</v>
       </c>
       <c r="H47" t="n">
-        <v>1.16</v>
+        <v>1.56</v>
       </c>
       <c r="I47" t="n">
-        <v>1.36</v>
+        <v>1.39</v>
       </c>
       <c r="J47" t="n">
-        <v>0.58</v>
+        <v>0.75</v>
       </c>
       <c r="K47" t="n">
-        <v>3.7</v>
+        <v>2.23</v>
       </c>
       <c r="L47" t="n">
-        <v>2.2</v>
+        <v>1.72</v>
       </c>
       <c r="M47" t="n">
-        <v>7.72</v>
+        <v>6.57</v>
       </c>
       <c r="N47" t="n">
-        <v>3.24</v>
+        <v>3.16</v>
       </c>
       <c r="O47" t="n">
-        <v>86.26</v>
+        <v>93.7</v>
       </c>
       <c r="P47" t="n">
-        <v>29.43</v>
+        <v>35.73</v>
       </c>
       <c r="Q47" t="n">
-        <v>0.67</v>
+        <v>0.78</v>
       </c>
       <c r="R47" t="n">
-        <v>0.88</v>
+        <v>1.12</v>
       </c>
       <c r="S47" t="n">
-        <v>141</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="48">
@@ -3337,55 +3337,55 @@
         <v>65</v>
       </c>
       <c r="B48" t="n">
-        <v>2.48</v>
+        <v>0.13</v>
       </c>
       <c r="C48" t="n">
-        <v>2.03</v>
+        <v>0.36</v>
       </c>
       <c r="D48" t="n">
-        <v>0.83</v>
+        <v>0.12</v>
       </c>
       <c r="E48" t="n">
-        <v>0.16</v>
+        <v>2.42</v>
       </c>
       <c r="F48" t="n">
-        <v>0.61</v>
+        <v>1.63</v>
       </c>
       <c r="G48" t="n">
-        <v>0.08</v>
+        <v>0.87</v>
       </c>
       <c r="H48" t="n">
-        <v>1.65</v>
+        <v>1.16</v>
       </c>
       <c r="I48" t="n">
-        <v>1.58</v>
+        <v>1.36</v>
       </c>
       <c r="J48" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="K48" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="L48" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="M48" t="n">
+        <v>7.72</v>
+      </c>
+      <c r="N48" t="n">
+        <v>3.24</v>
+      </c>
+      <c r="O48" t="n">
+        <v>86.26</v>
+      </c>
+      <c r="P48" t="n">
+        <v>29.43</v>
+      </c>
+      <c r="Q48" t="n">
         <v>0.67</v>
       </c>
-      <c r="K48" t="n">
-        <v>4.28</v>
-      </c>
-      <c r="L48" t="n">
-        <v>3</v>
-      </c>
-      <c r="M48" t="n">
-        <v>7.55</v>
-      </c>
-      <c r="N48" t="n">
-        <v>3.37</v>
-      </c>
-      <c r="O48" t="n">
-        <v>89.74</v>
-      </c>
-      <c r="P48" t="n">
-        <v>32.9</v>
-      </c>
-      <c r="Q48" t="n">
-        <v>1.06</v>
-      </c>
       <c r="R48" t="n">
-        <v>1.14</v>
+        <v>0.88</v>
       </c>
       <c r="S48" t="n">
         <v>141</v>
@@ -3396,58 +3396,58 @@
         <v>66</v>
       </c>
       <c r="B49" t="n">
-        <v>3.26</v>
+        <v>2.48</v>
       </c>
       <c r="C49" t="n">
-        <v>1.84</v>
+        <v>2.03</v>
       </c>
       <c r="D49" t="n">
-        <v>0.94</v>
+        <v>0.83</v>
       </c>
       <c r="E49" t="n">
-        <v>0.02</v>
+        <v>0.16</v>
       </c>
       <c r="F49" t="n">
-        <v>0.22</v>
+        <v>0.61</v>
       </c>
       <c r="G49" t="n">
-        <v>0.01</v>
+        <v>0.08</v>
       </c>
       <c r="H49" t="n">
-        <v>0.69</v>
+        <v>1.65</v>
       </c>
       <c r="I49" t="n">
-        <v>1.02</v>
+        <v>1.58</v>
       </c>
       <c r="J49" t="n">
-        <v>0.44</v>
+        <v>0.67</v>
       </c>
       <c r="K49" t="n">
-        <v>3.98</v>
+        <v>4.28</v>
       </c>
       <c r="L49" t="n">
-        <v>1.99</v>
+        <v>3</v>
       </c>
       <c r="M49" t="n">
-        <v>7.09</v>
+        <v>7.55</v>
       </c>
       <c r="N49" t="n">
-        <v>2.75</v>
+        <v>3.37</v>
       </c>
       <c r="O49" t="n">
-        <v>96.16</v>
+        <v>89.74</v>
       </c>
       <c r="P49" t="n">
-        <v>27.67</v>
+        <v>32.9</v>
       </c>
       <c r="Q49" t="n">
-        <v>0.86</v>
+        <v>1.06</v>
       </c>
       <c r="R49" t="n">
-        <v>0.98</v>
+        <v>1.14</v>
       </c>
       <c r="S49" t="n">
-        <v>81</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50">
@@ -3559,10 +3559,10 @@
         <v>46.33</v>
       </c>
       <c r="Q51" t="n">
-        <v>1.06</v>
+        <v>1.04</v>
       </c>
       <c r="R51" t="n">
-        <v>1.3</v>
+        <v>1.29</v>
       </c>
       <c r="S51" t="n">
         <v>143</v>

</xml_diff>